<commit_message>
Update week 2 schedule
</commit_message>
<xml_diff>
--- a/CMSC495_ProjectPlan.xlsx
+++ b/CMSC495_ProjectPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Git/CMSC495/cmsc495_final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Git/cmsc495_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3C9A43-2B1B-944B-9756-2718792A4194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A8D288-2AEF-B245-9591-BAA776EE031C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13780" yWindow="500" windowWidth="37420" windowHeight="25940" xr2:uid="{A3040AE0-0367-2B43-ADDE-84CCD12855DC}"/>
   </bookViews>
@@ -1153,72 +1153,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1242,6 +1176,72 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1637,48 +1637,48 @@
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="98" t="s">
+      <c r="M3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="96" t="s">
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="96"/>
-      <c r="U3" s="96"/>
-      <c r="V3" s="96"/>
-      <c r="W3" s="96"/>
-      <c r="X3" s="96"/>
-      <c r="Y3" s="97" t="s">
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="91"/>
+      <c r="X3" s="91"/>
+      <c r="Y3" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
+      <c r="Z3" s="75"/>
+      <c r="AA3" s="75"/>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="75"/>
+      <c r="AD3" s="75"/>
     </row>
     <row r="4" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="90"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="99" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101" t="s">
+      <c r="G4" s="78"/>
+      <c r="H4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103" t="s">
+      <c r="I4" s="80"/>
+      <c r="J4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="104"/>
+      <c r="K4" s="82"/>
       <c r="M4" s="12" t="str">
         <f>TEXT(M5,"aaa")</f>
         <v>Tue</v>
@@ -1973,13 +1973,13 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="D6" s="88" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="37">
-        <f t="shared" ref="N6:AQ16" si="2">IF($K6=N$5,3,IF(OR(AND($H6&lt;=N$5,N$5&lt;=$I6),$H6=N$5),2,IF(AND($F6&lt;=N$5,N$5&lt;=$G6),1,0)))</f>
+        <f t="shared" ref="N6:AQ6" si="2">IF($K6=N$5,3,IF(OR(AND($H6&lt;=N$5,N$5&lt;=$I6),$H6=N$5),2,IF(AND($F6&lt;=N$5,N$5&lt;=$G6),1,0)))</f>
         <v>0</v>
       </c>
       <c r="O6" s="37">
@@ -2130,9 +2130,9 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="85"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="95"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="89"/>
       <c r="E7" s="31" t="s">
         <v>13</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>44636</v>
       </c>
       <c r="M7" s="39">
-        <f t="shared" ref="M7:AB38" si="3">IF($K7=M$5,3,IF(OR(AND($H7&lt;=M$5,M$5&lt;=$I7),$H7=M$5),2,IF(AND($F7&lt;=M$5,M$5&lt;=$G7),1,0)))</f>
+        <f t="shared" ref="M7:AB22" si="3">IF($K7=M$5,3,IF(OR(AND($H7&lt;=M$5,M$5&lt;=$I7),$H7=M$5),2,IF(AND($F7&lt;=M$5,M$5&lt;=$G7),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N7" s="40">
@@ -2217,7 +2217,7 @@
         <v>3</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" ref="AC7:AQ70" si="4">IF($K7=AC$5,3,IF(OR(AND($H7&lt;=AC$5,AC$5&lt;=$I7),$H7=AC$5),2,IF(AND($F7&lt;=AC$5,AC$5&lt;=$G7),1,0)))</f>
+        <f t="shared" ref="AC7:AQ21" si="4">IF($K7=AC$5,3,IF(OR(AND($H7&lt;=AC$5,AC$5&lt;=$I7),$H7=AC$5),2,IF(AND($F7&lt;=AC$5,AC$5&lt;=$G7),1,0)))</f>
         <v>1</v>
       </c>
       <c r="AD7" s="40">
@@ -2281,9 +2281,9 @@
       </c>
     </row>
     <row r="8" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="85"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="95"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="89"/>
       <c r="E8" s="31" t="s">
         <v>15</v>
       </c>
@@ -2429,10 +2429,10 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="95" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="71" t="s">
@@ -2581,8 +2581,8 @@
       </c>
     </row>
     <row r="10" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="81"/>
-      <c r="C10" s="84"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="72" t="s">
         <v>62</v>
       </c>
@@ -2733,8 +2733,8 @@
       </c>
     </row>
     <row r="11" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="81"/>
-      <c r="C11" s="84"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="72" t="s">
         <v>62</v>
       </c>
@@ -2879,8 +2879,8 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="81"/>
-      <c r="C12" s="84"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="73" t="s">
         <v>70</v>
       </c>
@@ -2893,7 +2893,9 @@
       <c r="G12" s="33">
         <v>44645</v>
       </c>
-      <c r="H12" s="32"/>
+      <c r="H12" s="32">
+        <v>44643</v>
+      </c>
       <c r="I12" s="33"/>
       <c r="J12" s="34" t="s">
         <v>13</v>
@@ -2989,7 +2991,7 @@
       </c>
       <c r="AI12" s="40">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ12" s="40">
         <f t="shared" si="4"/>
@@ -3025,8 +3027,8 @@
       </c>
     </row>
     <row r="13" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="81"/>
-      <c r="C13" s="84"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="74" t="s">
         <v>58</v>
       </c>
@@ -3167,9 +3169,9 @@
       </c>
     </row>
     <row r="14" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="81"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="87" t="s">
+      <c r="B14" s="93"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="98" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="31" t="s">
@@ -3315,9 +3317,9 @@
       </c>
     </row>
     <row r="15" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="81"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="88"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="99"/>
       <c r="E15" s="31" t="s">
         <v>13</v>
       </c>
@@ -3463,9 +3465,9 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="82"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="89"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="100"/>
       <c r="E16" s="31" t="s">
         <v>15</v>
       </c>
@@ -3611,10 +3613,10 @@
       </c>
     </row>
     <row r="17" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="85"/>
+      <c r="C17" s="87"/>
       <c r="D17" s="66" t="s">
         <v>80</v>
       </c>
@@ -3753,8 +3755,8 @@
       </c>
     </row>
     <row r="18" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
       <c r="D18" s="44" t="s">
         <v>54</v>
       </c>
@@ -3893,8 +3895,8 @@
       </c>
     </row>
     <row r="19" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="85"/>
-      <c r="C19" s="85"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="44" t="s">
         <v>55</v>
       </c>
@@ -4033,8 +4035,8 @@
       </c>
     </row>
     <row r="20" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
       <c r="D20" s="44" t="s">
         <v>79</v>
       </c>
@@ -4173,8 +4175,8 @@
       </c>
     </row>
     <row r="21" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="85"/>
-      <c r="C21" s="85"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="67" t="s">
         <v>63</v>
       </c>
@@ -4313,8 +4315,8 @@
       </c>
     </row>
     <row r="22" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="85"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="45" t="s">
         <v>71</v>
       </c>
@@ -4392,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="40">
-        <f t="shared" ref="AB22:AQ73" si="5">IF($K22=AB$5,3,IF(OR(AND($H22&lt;=AB$5,AB$5&lt;=$I22),$H22=AB$5),2,IF(AND($F22&lt;=AB$5,AB$5&lt;=$G22),1,0)))</f>
+        <f t="shared" ref="AB22:AQ37" si="5">IF($K22=AB$5,3,IF(OR(AND($H22&lt;=AB$5,AB$5&lt;=$I22),$H22=AB$5),2,IF(AND($F22&lt;=AB$5,AB$5&lt;=$G22),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC22" s="40">
@@ -4457,8 +4459,8 @@
       </c>
     </row>
     <row r="23" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="67" t="s">
         <v>58</v>
       </c>
@@ -4474,7 +4476,7 @@
       <c r="J23" s="34"/>
       <c r="K23" s="35"/>
       <c r="M23" s="39">
-        <f t="shared" ref="M23:AB54" si="6">IF($K23=M$5,3,IF(OR(AND($H23&lt;=M$5,M$5&lt;=$I23),$H23=M$5),2,IF(AND($F23&lt;=M$5,M$5&lt;=$G23),1,0)))</f>
+        <f t="shared" ref="M23:AB38" si="6">IF($K23=M$5,3,IF(OR(AND($H23&lt;=M$5,M$5&lt;=$I23),$H23=M$5),2,IF(AND($F23&lt;=M$5,M$5&lt;=$G23),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N23" s="40">
@@ -4599,8 +4601,8 @@
       </c>
     </row>
     <row r="24" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="85"/>
-      <c r="C24" s="85"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="67" t="s">
         <v>77</v>
       </c>
@@ -4743,8 +4745,8 @@
       </c>
     </row>
     <row r="25" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="86"/>
-      <c r="C25" s="85"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="87"/>
       <c r="D25" s="46" t="s">
         <v>17</v>
       </c>
@@ -4888,7 +4890,7 @@
     </row>
     <row r="26" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="61"/>
-      <c r="C26" s="85"/>
+      <c r="C26" s="87"/>
       <c r="D26" s="43" t="s">
         <v>64</v>
       </c>
@@ -5027,10 +5029,10 @@
       </c>
     </row>
     <row r="27" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="85"/>
+      <c r="C27" s="87"/>
       <c r="D27" s="44" t="s">
         <v>38</v>
       </c>
@@ -5169,8 +5171,8 @@
       </c>
     </row>
     <row r="28" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="85"/>
-      <c r="C28" s="85"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="87"/>
       <c r="D28" s="44" t="s">
         <v>68</v>
       </c>
@@ -5309,8 +5311,8 @@
       </c>
     </row>
     <row r="29" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="85"/>
-      <c r="C29" s="85"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="44" t="s">
         <v>39</v>
       </c>
@@ -5449,8 +5451,8 @@
       </c>
     </row>
     <row r="30" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="85"/>
-      <c r="C30" s="85"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="87"/>
       <c r="D30" s="44" t="s">
         <v>40</v>
       </c>
@@ -5589,8 +5591,8 @@
       </c>
     </row>
     <row r="31" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="44" t="s">
         <v>65</v>
       </c>
@@ -5727,8 +5729,8 @@
       </c>
     </row>
     <row r="32" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="85"/>
-      <c r="C32" s="85"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="87"/>
       <c r="D32" s="44" t="s">
         <v>69</v>
       </c>
@@ -5867,8 +5869,8 @@
       </c>
     </row>
     <row r="33" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="85"/>
-      <c r="C33" s="85"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="87"/>
       <c r="D33" s="45" t="s">
         <v>72</v>
       </c>
@@ -6011,8 +6013,8 @@
       </c>
     </row>
     <row r="34" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="85"/>
-      <c r="C34" s="85"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
       <c r="D34" s="67" t="s">
         <v>58</v>
       </c>
@@ -6153,8 +6155,8 @@
       </c>
     </row>
     <row r="35" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="85"/>
-      <c r="C35" s="85"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="87"/>
       <c r="D35" s="44" t="s">
         <v>41</v>
       </c>
@@ -6297,8 +6299,8 @@
       </c>
     </row>
     <row r="36" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
       <c r="D36" s="45" t="s">
         <v>18</v>
       </c>
@@ -6441,10 +6443,10 @@
       </c>
     </row>
     <row r="37" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="79" t="s">
+      <c r="C37" s="104" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="43" t="s">
@@ -6585,8 +6587,8 @@
       </c>
     </row>
     <row r="38" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="76"/>
-      <c r="C38" s="79"/>
+      <c r="B38" s="102"/>
+      <c r="C38" s="104"/>
       <c r="D38" s="66" t="s">
         <v>42</v>
       </c>
@@ -6660,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="40">
-        <f t="shared" ref="AB38:AQ73" si="7">IF($K38=AB$5,3,IF(OR(AND($H38&lt;=AB$5,AB$5&lt;=$I38),$H38=AB$5),2,IF(AND($F38&lt;=AB$5,AB$5&lt;=$G38),1,0)))</f>
+        <f t="shared" ref="AB38:AQ53" si="7">IF($K38=AB$5,3,IF(OR(AND($H38&lt;=AB$5,AB$5&lt;=$I38),$H38=AB$5),2,IF(AND($F38&lt;=AB$5,AB$5&lt;=$G38),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC38" s="40">
@@ -6725,8 +6727,8 @@
       </c>
     </row>
     <row r="39" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="76"/>
-      <c r="C39" s="79"/>
+      <c r="B39" s="102"/>
+      <c r="C39" s="104"/>
       <c r="D39" s="66" t="s">
         <v>67</v>
       </c>
@@ -6738,7 +6740,7 @@
       <c r="J39" s="34"/>
       <c r="K39" s="35"/>
       <c r="M39" s="39">
-        <f t="shared" ref="M39:AB73" si="8">IF($K39=M$5,3,IF(OR(AND($H39&lt;=M$5,M$5&lt;=$I39),$H39=M$5),2,IF(AND($F39&lt;=M$5,M$5&lt;=$G39),1,0)))</f>
+        <f t="shared" ref="M39:AB54" si="8">IF($K39=M$5,3,IF(OR(AND($H39&lt;=M$5,M$5&lt;=$I39),$H39=M$5),2,IF(AND($F39&lt;=M$5,M$5&lt;=$G39),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N39" s="40">
@@ -6863,8 +6865,8 @@
       </c>
     </row>
     <row r="40" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="76"/>
-      <c r="C40" s="79"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="104"/>
       <c r="D40" s="44" t="s">
         <v>46</v>
       </c>
@@ -7003,8 +7005,8 @@
       </c>
     </row>
     <row r="41" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="76"/>
-      <c r="C41" s="79"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="104"/>
       <c r="D41" s="45" t="s">
         <v>73</v>
       </c>
@@ -7147,8 +7149,8 @@
       </c>
     </row>
     <row r="42" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="76"/>
-      <c r="C42" s="79"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="104"/>
       <c r="D42" s="67" t="s">
         <v>58</v>
       </c>
@@ -7289,8 +7291,8 @@
       </c>
     </row>
     <row r="43" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="76"/>
-      <c r="C43" s="79"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="104"/>
       <c r="D43" s="47" t="s">
         <v>19</v>
       </c>
@@ -7433,8 +7435,8 @@
       </c>
     </row>
     <row r="44" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="76"/>
-      <c r="C44" s="79"/>
+      <c r="B44" s="102"/>
+      <c r="C44" s="104"/>
       <c r="D44" s="47" t="s">
         <v>48</v>
       </c>
@@ -7577,8 +7579,8 @@
       </c>
     </row>
     <row r="45" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="76"/>
-      <c r="C45" s="79"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="104"/>
       <c r="D45" s="45" t="s">
         <v>48</v>
       </c>
@@ -7721,8 +7723,8 @@
       </c>
     </row>
     <row r="46" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="77"/>
-      <c r="C46" s="79"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="104"/>
       <c r="D46" s="65" t="s">
         <v>50</v>
       </c>
@@ -7863,10 +7865,10 @@
       </c>
     </row>
     <row r="47" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="75" t="s">
+      <c r="B47" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="79"/>
+      <c r="C47" s="104"/>
       <c r="D47" s="66" t="s">
         <v>39</v>
       </c>
@@ -8005,8 +8007,8 @@
       </c>
     </row>
     <row r="48" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="76"/>
-      <c r="C48" s="79"/>
+      <c r="B48" s="102"/>
+      <c r="C48" s="104"/>
       <c r="D48" s="44" t="s">
         <v>40</v>
       </c>
@@ -8145,8 +8147,8 @@
       </c>
     </row>
     <row r="49" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="76"/>
-      <c r="C49" s="79"/>
+      <c r="B49" s="102"/>
+      <c r="C49" s="104"/>
       <c r="D49" s="44" t="s">
         <v>47</v>
       </c>
@@ -8285,8 +8287,8 @@
       </c>
     </row>
     <row r="50" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="76"/>
-      <c r="C50" s="79"/>
+      <c r="B50" s="102"/>
+      <c r="C50" s="104"/>
       <c r="D50" s="44" t="s">
         <v>49</v>
       </c>
@@ -8423,8 +8425,8 @@
       </c>
     </row>
     <row r="51" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="76"/>
-      <c r="C51" s="79"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="104"/>
       <c r="D51" s="45" t="s">
         <v>74</v>
       </c>
@@ -8567,8 +8569,8 @@
       </c>
     </row>
     <row r="52" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="76"/>
-      <c r="C52" s="79"/>
+      <c r="B52" s="102"/>
+      <c r="C52" s="104"/>
       <c r="D52" s="67" t="s">
         <v>58</v>
       </c>
@@ -8709,8 +8711,8 @@
       </c>
     </row>
     <row r="53" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="76"/>
-      <c r="C53" s="79"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="104"/>
       <c r="D53" s="47" t="s">
         <v>20</v>
       </c>
@@ -8849,8 +8851,8 @@
       </c>
     </row>
     <row r="54" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="76"/>
-      <c r="C54" s="79"/>
+      <c r="B54" s="102"/>
+      <c r="C54" s="104"/>
       <c r="D54" s="47" t="s">
         <v>44</v>
       </c>
@@ -8924,7 +8926,7 @@
         <v>0</v>
       </c>
       <c r="AB54" s="40">
-        <f t="shared" ref="AB54:AQ73" si="9">IF($K54=AB$5,3,IF(OR(AND($H54&lt;=AB$5,AB$5&lt;=$I54),$H54=AB$5),2,IF(AND($F54&lt;=AB$5,AB$5&lt;=$G54),1,0)))</f>
+        <f t="shared" ref="AB54:AQ69" si="9">IF($K54=AB$5,3,IF(OR(AND($H54&lt;=AB$5,AB$5&lt;=$I54),$H54=AB$5),2,IF(AND($F54&lt;=AB$5,AB$5&lt;=$G54),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC54" s="40">
@@ -8989,8 +8991,8 @@
       </c>
     </row>
     <row r="55" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="77"/>
-      <c r="C55" s="79"/>
+      <c r="B55" s="103"/>
+      <c r="C55" s="104"/>
       <c r="D55" s="46" t="s">
         <v>44</v>
       </c>
@@ -9008,7 +9010,7 @@
       <c r="J55" s="34"/>
       <c r="K55" s="35"/>
       <c r="M55" s="39">
-        <f t="shared" ref="M55:AB73" si="10">IF($K55=M$5,3,IF(OR(AND($H55&lt;=M$5,M$5&lt;=$I55),$H55=M$5),2,IF(AND($F55&lt;=M$5,M$5&lt;=$G55),1,0)))</f>
+        <f t="shared" ref="M55:AB70" si="10">IF($K55=M$5,3,IF(OR(AND($H55&lt;=M$5,M$5&lt;=$I55),$H55=M$5),2,IF(AND($F55&lt;=M$5,M$5&lt;=$G55),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N55" s="40">
@@ -9133,10 +9135,10 @@
       </c>
     </row>
     <row r="56" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="78" t="s">
+      <c r="C56" s="90" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="43" t="s">
@@ -9277,8 +9279,8 @@
       </c>
     </row>
     <row r="57" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="76"/>
-      <c r="C57" s="78"/>
+      <c r="B57" s="102"/>
+      <c r="C57" s="90"/>
       <c r="D57" s="50" t="s">
         <v>59</v>
       </c>
@@ -9415,8 +9417,8 @@
       </c>
     </row>
     <row r="58" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="76"/>
-      <c r="C58" s="78"/>
+      <c r="B58" s="102"/>
+      <c r="C58" s="90"/>
       <c r="D58" s="51" t="s">
         <v>60</v>
       </c>
@@ -9553,8 +9555,8 @@
       </c>
     </row>
     <row r="59" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="76"/>
-      <c r="C59" s="78"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="90"/>
       <c r="D59" s="30" t="s">
         <v>43</v>
       </c>
@@ -9691,8 +9693,8 @@
       </c>
     </row>
     <row r="60" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="76"/>
-      <c r="C60" s="78"/>
+      <c r="B60" s="102"/>
+      <c r="C60" s="90"/>
       <c r="D60" s="44" t="s">
         <v>50</v>
       </c>
@@ -9829,8 +9831,8 @@
       </c>
     </row>
     <row r="61" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="76"/>
-      <c r="C61" s="78"/>
+      <c r="B61" s="102"/>
+      <c r="C61" s="90"/>
       <c r="D61" s="44" t="s">
         <v>61</v>
       </c>
@@ -9967,8 +9969,8 @@
       </c>
     </row>
     <row r="62" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="76"/>
-      <c r="C62" s="78"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="90"/>
       <c r="D62" s="45" t="s">
         <v>75</v>
       </c>
@@ -10111,8 +10113,8 @@
       </c>
     </row>
     <row r="63" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="76"/>
-      <c r="C63" s="78"/>
+      <c r="B63" s="102"/>
+      <c r="C63" s="90"/>
       <c r="D63" s="67" t="s">
         <v>58</v>
       </c>
@@ -10253,8 +10255,8 @@
       </c>
     </row>
     <row r="64" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="76"/>
-      <c r="C64" s="78"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="90"/>
       <c r="D64" s="47" t="s">
         <v>21</v>
       </c>
@@ -10393,8 +10395,8 @@
       </c>
     </row>
     <row r="65" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="76"/>
-      <c r="C65" s="78"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="90"/>
       <c r="D65" s="52" t="s">
         <v>45</v>
       </c>
@@ -10533,8 +10535,8 @@
       </c>
     </row>
     <row r="66" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="76"/>
-      <c r="C66" s="78"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="90"/>
       <c r="D66" s="53" t="s">
         <v>45</v>
       </c>
@@ -10677,10 +10679,10 @@
       </c>
     </row>
     <row r="67" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="75" t="s">
+      <c r="B67" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="78" t="s">
+      <c r="C67" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D67" s="50" t="s">
@@ -10819,8 +10821,8 @@
       </c>
     </row>
     <row r="68" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="76"/>
-      <c r="C68" s="78"/>
+      <c r="B68" s="102"/>
+      <c r="C68" s="90"/>
       <c r="D68" s="30" t="s">
         <v>34</v>
       </c>
@@ -10958,8 +10960,8 @@
       </c>
     </row>
     <row r="69" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="76"/>
-      <c r="C69" s="78"/>
+      <c r="B69" s="102"/>
+      <c r="C69" s="90"/>
       <c r="D69" s="30" t="s">
         <v>34</v>
       </c>
@@ -11098,8 +11100,8 @@
       </c>
     </row>
     <row r="70" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="76"/>
-      <c r="C70" s="78"/>
+      <c r="B70" s="102"/>
+      <c r="C70" s="90"/>
       <c r="D70" s="30" t="s">
         <v>34</v>
       </c>
@@ -11238,8 +11240,8 @@
       </c>
     </row>
     <row r="71" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="76"/>
-      <c r="C71" s="78"/>
+      <c r="B71" s="102"/>
+      <c r="C71" s="90"/>
       <c r="D71" s="69" t="s">
         <v>76</v>
       </c>
@@ -11380,8 +11382,8 @@
       </c>
     </row>
     <row r="72" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="76"/>
-      <c r="C72" s="78"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="90"/>
       <c r="D72" s="30" t="s">
         <v>58</v>
       </c>
@@ -11522,8 +11524,8 @@
       </c>
     </row>
     <row r="73" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="77"/>
-      <c r="C73" s="78"/>
+      <c r="B73" s="103"/>
+      <c r="C73" s="90"/>
       <c r="D73" s="54" t="s">
         <v>57</v>
       </c>
@@ -11666,21 +11668,6 @@
   </sheetData>
   <autoFilter ref="D5:E73" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}"/>
   <mergeCells count="22">
-    <mergeCell ref="Y3:AD3"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="S3:X3"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="C9:C36"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="B27:B36"/>
     <mergeCell ref="B67:B73"/>
     <mergeCell ref="C67:C73"/>
     <mergeCell ref="B37:B46"/>
@@ -11688,6 +11675,21 @@
     <mergeCell ref="B47:B55"/>
     <mergeCell ref="B56:B66"/>
     <mergeCell ref="C56:C66"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="C9:C36"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="B27:B36"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="Y3:AD3"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="M6:AQ73">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Updated week5 to week8
</commit_message>
<xml_diff>
--- a/CMSC495_ProjectPlan.xlsx
+++ b/CMSC495_ProjectPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Git/cmsc495_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B901CEE5-161D-B34C-AEB5-9F7E4C7B5B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E85E297-65E4-3740-AF07-D1C00A1CCA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19860" yWindow="500" windowWidth="51200" windowHeight="26260" xr2:uid="{A3040AE0-0367-2B43-ADDE-84CCD12855DC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26260" xr2:uid="{A3040AE0-0367-2B43-ADDE-84CCD12855DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Plan" sheetId="1" r:id="rId1"/>
@@ -1353,102 +1353,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1479,6 +1383,102 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1817,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}">
   <dimension ref="A1:AV94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1874,48 +1874,48 @@
       <c r="D3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="78" t="s">
+      <c r="M3" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="93" t="s">
+      <c r="N3" s="114"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="93"/>
-      <c r="U3" s="93"/>
-      <c r="V3" s="93"/>
-      <c r="W3" s="93"/>
-      <c r="X3" s="93"/>
-      <c r="Y3" s="77" t="s">
+      <c r="T3" s="112"/>
+      <c r="U3" s="112"/>
+      <c r="V3" s="112"/>
+      <c r="W3" s="112"/>
+      <c r="X3" s="112"/>
+      <c r="Y3" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="77"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="77"/>
+      <c r="Z3" s="113"/>
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113"/>
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="113"/>
     </row>
     <row r="4" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="79" t="s">
+      <c r="B4" s="105"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="81" t="s">
+      <c r="G4" s="116"/>
+      <c r="H4" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="82"/>
-      <c r="J4" s="83" t="s">
+      <c r="I4" s="118"/>
+      <c r="J4" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="84"/>
+      <c r="K4" s="120"/>
       <c r="M4" s="12" t="str">
         <f>TEXT(M5,"aaa")</f>
         <v>Fri</v>
@@ -2210,13 +2210,13 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="108" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="110" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="37">
-        <f t="shared" ref="N6:AQ14" si="2">IF($K6=N$5,3,IF(OR(AND($H6&lt;=N$5,N$5&lt;=$I6),$H6=N$5),2,IF(AND($F6&lt;=N$5,N$5&lt;=$G6),1,0)))</f>
+        <f t="shared" ref="N6:AQ6" si="2">IF($K6=N$5,3,IF(OR(AND($H6&lt;=N$5,N$5&lt;=$I6),$H6=N$5),2,IF(AND($F6&lt;=N$5,N$5&lt;=$G6),1,0)))</f>
         <v>0</v>
       </c>
       <c r="O6" s="37">
@@ -2367,9 +2367,9 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="89"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="92"/>
-      <c r="D7" s="91"/>
+      <c r="D7" s="111"/>
       <c r="E7" s="31" t="s">
         <v>13</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>44636</v>
       </c>
       <c r="M7" s="39">
-        <f t="shared" ref="M7:AB38" si="3">IF($K7=M$5,3,IF(OR(AND($H7&lt;=M$5,M$5&lt;=$I7),$H7=M$5),2,IF(AND($F7&lt;=M$5,M$5&lt;=$G7),1,0)))</f>
+        <f t="shared" ref="M7:AB22" si="3">IF($K7=M$5,3,IF(OR(AND($H7&lt;=M$5,M$5&lt;=$I7),$H7=M$5),2,IF(AND($F7&lt;=M$5,M$5&lt;=$G7),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N7" s="40">
@@ -2454,7 +2454,7 @@
         <v>0</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" ref="AC7:AQ70" si="4">IF($K7=AC$5,3,IF(OR(AND($H7&lt;=AC$5,AC$5&lt;=$I7),$H7=AC$5),2,IF(AND($F7&lt;=AC$5,AC$5&lt;=$G7),1,0)))</f>
+        <f t="shared" ref="AC7:AQ21" si="4">IF($K7=AC$5,3,IF(OR(AND($H7&lt;=AC$5,AC$5&lt;=$I7),$H7=AC$5),2,IF(AND($F7&lt;=AC$5,AC$5&lt;=$G7),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AD7" s="40">
@@ -2518,9 +2518,9 @@
       </c>
     </row>
     <row r="8" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="89"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="92"/>
-      <c r="D8" s="91"/>
+      <c r="D8" s="111"/>
       <c r="E8" s="31" t="s">
         <v>15</v>
       </c>
@@ -2666,10 +2666,10 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="C9" s="100" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="64" t="s">
@@ -2822,8 +2822,8 @@
       </c>
     </row>
     <row r="10" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="95"/>
-      <c r="C10" s="97"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="101"/>
       <c r="D10" s="65" t="s">
         <v>49</v>
       </c>
@@ -2974,8 +2974,8 @@
       </c>
     </row>
     <row r="11" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="95"/>
-      <c r="C11" s="97"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="101"/>
       <c r="D11" s="65" t="s">
         <v>49</v>
       </c>
@@ -3126,8 +3126,8 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="95"/>
-      <c r="C12" s="97"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="101"/>
       <c r="D12" s="66" t="s">
         <v>52</v>
       </c>
@@ -3278,8 +3278,8 @@
       </c>
     </row>
     <row r="13" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="95"/>
-      <c r="C13" s="97"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="101"/>
       <c r="D13" s="67" t="s">
         <v>48</v>
       </c>
@@ -3428,9 +3428,9 @@
       </c>
     </row>
     <row r="14" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="95"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="99" t="s">
+      <c r="B14" s="99"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="103" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="31" t="s">
@@ -3576,9 +3576,9 @@
       </c>
     </row>
     <row r="15" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="95"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="100"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="104"/>
       <c r="E15" s="31" t="s">
         <v>13</v>
       </c>
@@ -3726,9 +3726,9 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="95"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="100"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="104"/>
       <c r="E16" s="31" t="s">
         <v>15</v>
       </c>
@@ -3876,10 +3876,10 @@
       </c>
     </row>
     <row r="17" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="97"/>
+      <c r="C17" s="101"/>
       <c r="D17" s="72" t="s">
         <v>61</v>
       </c>
@@ -4030,8 +4030,8 @@
       </c>
     </row>
     <row r="18" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="95"/>
-      <c r="C18" s="97"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="101"/>
       <c r="D18" s="73" t="s">
         <v>63</v>
       </c>
@@ -4182,8 +4182,8 @@
       </c>
     </row>
     <row r="19" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="95"/>
-      <c r="C19" s="97"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="74" t="s">
         <v>44</v>
       </c>
@@ -4334,8 +4334,8 @@
       </c>
     </row>
     <row r="20" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="95"/>
-      <c r="C20" s="97"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="101"/>
       <c r="D20" s="74" t="s">
         <v>45</v>
       </c>
@@ -4486,8 +4486,8 @@
       </c>
     </row>
     <row r="21" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="95"/>
-      <c r="C21" s="97"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="101"/>
       <c r="D21" s="74" t="s">
         <v>62</v>
       </c>
@@ -4638,8 +4638,8 @@
       </c>
     </row>
     <row r="22" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="95"/>
-      <c r="C22" s="97"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="101"/>
       <c r="D22" s="75" t="s">
         <v>64</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="40">
-        <f t="shared" ref="AB22:AQ85" si="5">IF($K22=AB$5,3,IF(OR(AND($H22&lt;=AB$5,AB$5&lt;=$I22),$H22=AB$5),2,IF(AND($F22&lt;=AB$5,AB$5&lt;=$G22),1,0)))</f>
+        <f t="shared" ref="AB22:AQ37" si="5">IF($K22=AB$5,3,IF(OR(AND($H22&lt;=AB$5,AB$5&lt;=$I22),$H22=AB$5),2,IF(AND($F22&lt;=AB$5,AB$5&lt;=$G22),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC22" s="40">
@@ -4790,8 +4790,8 @@
       </c>
     </row>
     <row r="23" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="95"/>
-      <c r="C23" s="97"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="75" t="s">
         <v>50</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>44651</v>
       </c>
       <c r="M23" s="39">
-        <f t="shared" ref="M23:AB54" si="6">IF($K23=M$5,3,IF(OR(AND($H23&lt;=M$5,M$5&lt;=$I23),$H23=M$5),2,IF(AND($F23&lt;=M$5,M$5&lt;=$G23),1,0)))</f>
+        <f t="shared" ref="M23:AB38" si="6">IF($K23=M$5,3,IF(OR(AND($H23&lt;=M$5,M$5&lt;=$I23),$H23=M$5),2,IF(AND($F23&lt;=M$5,M$5&lt;=$G23),1,0)))</f>
         <v>1</v>
       </c>
       <c r="N23" s="40">
@@ -4942,8 +4942,8 @@
       </c>
     </row>
     <row r="24" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="95"/>
-      <c r="C24" s="97"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="101"/>
       <c r="D24" s="76" t="s">
         <v>53</v>
       </c>
@@ -5094,8 +5094,8 @@
       </c>
     </row>
     <row r="25" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="95"/>
-      <c r="C25" s="97"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="75" t="s">
         <v>48</v>
       </c>
@@ -5244,8 +5244,8 @@
       </c>
     </row>
     <row r="26" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="95"/>
-      <c r="C26" s="97"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="101"/>
       <c r="D26" s="75" t="s">
         <v>59</v>
       </c>
@@ -5396,8 +5396,8 @@
       </c>
     </row>
     <row r="27" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="95"/>
-      <c r="C27" s="97"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="101"/>
       <c r="D27" s="76" t="s">
         <v>17</v>
       </c>
@@ -5548,10 +5548,10 @@
       </c>
     </row>
     <row r="28" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="97"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="72" t="s">
         <v>51</v>
       </c>
@@ -5702,8 +5702,8 @@
       </c>
     </row>
     <row r="29" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="95"/>
-      <c r="C29" s="97"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="101"/>
       <c r="D29" s="74" t="s">
         <v>38</v>
       </c>
@@ -5854,8 +5854,8 @@
       </c>
     </row>
     <row r="30" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="95"/>
-      <c r="C30" s="97"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="101"/>
       <c r="D30" s="74" t="s">
         <v>65</v>
       </c>
@@ -6006,8 +6006,8 @@
       </c>
     </row>
     <row r="31" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="95"/>
-      <c r="C31" s="97"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="74" t="s">
         <v>39</v>
       </c>
@@ -6158,8 +6158,8 @@
       </c>
     </row>
     <row r="32" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="95"/>
-      <c r="C32" s="97"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="101"/>
       <c r="D32" s="74" t="s">
         <v>40</v>
       </c>
@@ -6310,8 +6310,8 @@
       </c>
     </row>
     <row r="33" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="95"/>
-      <c r="C33" s="97"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="101"/>
       <c r="D33" s="74" t="s">
         <v>66</v>
       </c>
@@ -6462,8 +6462,8 @@
       </c>
     </row>
     <row r="34" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="95"/>
-      <c r="C34" s="97"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="101"/>
       <c r="D34" s="74" t="s">
         <v>67</v>
       </c>
@@ -6614,8 +6614,8 @@
       </c>
     </row>
     <row r="35" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="95"/>
-      <c r="C35" s="97"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="101"/>
       <c r="D35" s="76" t="s">
         <v>54</v>
       </c>
@@ -6766,8 +6766,8 @@
       </c>
     </row>
     <row r="36" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="95"/>
-      <c r="C36" s="97"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="101"/>
       <c r="D36" s="75" t="s">
         <v>48</v>
       </c>
@@ -6916,8 +6916,8 @@
       </c>
     </row>
     <row r="37" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="95"/>
-      <c r="C37" s="97"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="101"/>
       <c r="D37" s="74" t="s">
         <v>41</v>
       </c>
@@ -7068,8 +7068,8 @@
       </c>
     </row>
     <row r="38" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="95"/>
-      <c r="C38" s="98"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="102"/>
       <c r="D38" s="76" t="s">
         <v>18</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="40">
-        <f t="shared" ref="AB38:AQ94" si="7">IF($K38=AB$5,3,IF(OR(AND($H38&lt;=AB$5,AB$5&lt;=$I38),$H38=AB$5),2,IF(AND($F38&lt;=AB$5,AB$5&lt;=$G38),1,0)))</f>
+        <f t="shared" ref="AB38:AQ53" si="7">IF($K38=AB$5,3,IF(OR(AND($H38&lt;=AB$5,AB$5&lt;=$I38),$H38=AB$5),2,IF(AND($F38&lt;=AB$5,AB$5&lt;=$G38),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC38" s="40">
@@ -7220,10 +7220,10 @@
       </c>
     </row>
     <row r="39" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="108" t="s">
+      <c r="C39" s="96" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="68" t="s">
@@ -7245,7 +7245,7 @@
       </c>
       <c r="K39" s="35"/>
       <c r="M39" s="39">
-        <f t="shared" ref="M39:AB70" si="8">IF($K39=M$5,3,IF(OR(AND($H39&lt;=M$5,M$5&lt;=$I39),$H39=M$5),2,IF(AND($F39&lt;=M$5,M$5&lt;=$G39),1,0)))</f>
+        <f t="shared" ref="M39:AB54" si="8">IF($K39=M$5,3,IF(OR(AND($H39&lt;=M$5,M$5&lt;=$I39),$H39=M$5),2,IF(AND($F39&lt;=M$5,M$5&lt;=$G39),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N39" s="40">
@@ -7370,9 +7370,9 @@
       </c>
     </row>
     <row r="40" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="106"/>
-      <c r="C40" s="108"/>
-      <c r="D40" s="109" t="s">
+      <c r="B40" s="94"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="77" t="s">
         <v>73</v>
       </c>
       <c r="E40" s="31" t="s">
@@ -7516,9 +7516,9 @@
       </c>
     </row>
     <row r="41" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="106"/>
-      <c r="C41" s="108"/>
-      <c r="D41" s="109" t="s">
+      <c r="B41" s="94"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="77" t="s">
         <v>69</v>
       </c>
       <c r="E41" s="31" t="s">
@@ -7662,8 +7662,8 @@
       </c>
     </row>
     <row r="42" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="106"/>
-      <c r="C42" s="108"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="96"/>
       <c r="D42" s="69" t="s">
         <v>70</v>
       </c>
@@ -7808,8 +7808,8 @@
       </c>
     </row>
     <row r="43" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="106"/>
-      <c r="C43" s="108"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="96"/>
       <c r="D43" s="71" t="s">
         <v>55</v>
       </c>
@@ -7954,8 +7954,8 @@
       </c>
     </row>
     <row r="44" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="106"/>
-      <c r="C44" s="108"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="96"/>
       <c r="D44" s="70" t="s">
         <v>48</v>
       </c>
@@ -8098,9 +8098,9 @@
       </c>
     </row>
     <row r="45" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="106"/>
-      <c r="C45" s="108"/>
-      <c r="D45" s="110" t="s">
+      <c r="B45" s="94"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="78" t="s">
         <v>19</v>
       </c>
       <c r="E45" s="31" t="s">
@@ -8244,9 +8244,9 @@
       </c>
     </row>
     <row r="46" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="106"/>
-      <c r="C46" s="108"/>
-      <c r="D46" s="112" t="s">
+      <c r="B46" s="94"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="80" t="s">
         <v>72</v>
       </c>
       <c r="E46" s="31" t="s">
@@ -8390,9 +8390,9 @@
       </c>
     </row>
     <row r="47" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="106"/>
-      <c r="C47" s="108"/>
-      <c r="D47" s="113" t="s">
+      <c r="B47" s="94"/>
+      <c r="C47" s="96"/>
+      <c r="D47" s="81" t="s">
         <v>72</v>
       </c>
       <c r="E47" s="31" t="s">
@@ -8536,9 +8536,9 @@
       </c>
     </row>
     <row r="48" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="107"/>
-      <c r="C48" s="108"/>
-      <c r="D48" s="114" t="s">
+      <c r="B48" s="95"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="82" t="s">
         <v>72</v>
       </c>
       <c r="E48" s="31" t="s">
@@ -8682,10 +8682,10 @@
       </c>
     </row>
     <row r="49" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="102" t="s">
+      <c r="B49" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="104"/>
+      <c r="C49" s="97"/>
       <c r="D49" s="59" t="s">
         <v>75</v>
       </c>
@@ -8830,8 +8830,8 @@
       </c>
     </row>
     <row r="50" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="102"/>
-      <c r="C50" s="104"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="97"/>
       <c r="D50" s="44" t="s">
         <v>74</v>
       </c>
@@ -8976,8 +8976,8 @@
       </c>
     </row>
     <row r="51" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="102"/>
-      <c r="C51" s="104"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="97"/>
       <c r="D51" s="44" t="s">
         <v>76</v>
       </c>
@@ -9122,8 +9122,8 @@
       </c>
     </row>
     <row r="52" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="102"/>
-      <c r="C52" s="104"/>
+      <c r="B52" s="90"/>
+      <c r="C52" s="97"/>
       <c r="D52" s="44" t="s">
         <v>78</v>
       </c>
@@ -9268,8 +9268,8 @@
       </c>
     </row>
     <row r="53" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="102"/>
-      <c r="C53" s="104"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="97"/>
       <c r="D53" s="44" t="s">
         <v>79</v>
       </c>
@@ -9414,8 +9414,8 @@
       </c>
     </row>
     <row r="54" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="102"/>
-      <c r="C54" s="104"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="97"/>
       <c r="D54" s="44" t="s">
         <v>80</v>
       </c>
@@ -9495,7 +9495,7 @@
         <v>0</v>
       </c>
       <c r="AB54" s="40">
-        <f t="shared" ref="AB54:AQ94" si="9">IF($K54=AB$5,3,IF(OR(AND($H54&lt;=AB$5,AB$5&lt;=$I54),$H54=AB$5),2,IF(AND($F54&lt;=AB$5,AB$5&lt;=$G54),1,0)))</f>
+        <f t="shared" ref="AB54:AQ69" si="9">IF($K54=AB$5,3,IF(OR(AND($H54&lt;=AB$5,AB$5&lt;=$I54),$H54=AB$5),2,IF(AND($F54&lt;=AB$5,AB$5&lt;=$G54),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC54" s="40">
@@ -9560,8 +9560,8 @@
       </c>
     </row>
     <row r="55" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="102"/>
-      <c r="C55" s="104"/>
+      <c r="B55" s="90"/>
+      <c r="C55" s="97"/>
       <c r="D55" s="44" t="s">
         <v>77</v>
       </c>
@@ -9581,7 +9581,7 @@
       </c>
       <c r="K55" s="35"/>
       <c r="M55" s="39">
-        <f t="shared" ref="M55:AB94" si="10">IF($K55=M$5,3,IF(OR(AND($H55&lt;=M$5,M$5&lt;=$I55),$H55=M$5),2,IF(AND($F55&lt;=M$5,M$5&lt;=$G55),1,0)))</f>
+        <f t="shared" ref="M55:AB70" si="10">IF($K55=M$5,3,IF(OR(AND($H55&lt;=M$5,M$5&lt;=$I55),$H55=M$5),2,IF(AND($F55&lt;=M$5,M$5&lt;=$G55),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N55" s="40">
@@ -9706,8 +9706,8 @@
       </c>
     </row>
     <row r="56" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="102"/>
-      <c r="C56" s="104"/>
+      <c r="B56" s="90"/>
+      <c r="C56" s="97"/>
       <c r="D56" s="44" t="s">
         <v>81</v>
       </c>
@@ -9852,8 +9852,8 @@
       </c>
     </row>
     <row r="57" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="102"/>
-      <c r="C57" s="104"/>
+      <c r="B57" s="90"/>
+      <c r="C57" s="97"/>
       <c r="D57" s="60" t="s">
         <v>82</v>
       </c>
@@ -9998,8 +9998,8 @@
       </c>
     </row>
     <row r="58" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="102"/>
-      <c r="C58" s="104"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="97"/>
       <c r="D58" s="45" t="s">
         <v>56</v>
       </c>
@@ -10142,8 +10142,8 @@
       </c>
     </row>
     <row r="59" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="102"/>
-      <c r="C59" s="104"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="97"/>
       <c r="D59" s="60" t="s">
         <v>48</v>
       </c>
@@ -10286,13 +10286,13 @@
       </c>
     </row>
     <row r="60" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="102"/>
-      <c r="C60" s="104"/>
+      <c r="B60" s="90"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="46" t="s">
         <v>20</v>
       </c>
       <c r="E60" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F60" s="32"/>
       <c r="G60" s="35"/>
@@ -10426,9 +10426,9 @@
       </c>
     </row>
     <row r="61" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="102"/>
-      <c r="C61" s="104"/>
-      <c r="D61" s="115" t="s">
+      <c r="B61" s="90"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="83" t="s">
         <v>72</v>
       </c>
       <c r="E61" s="31" t="s">
@@ -10572,9 +10572,9 @@
       </c>
     </row>
     <row r="62" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="102"/>
-      <c r="C62" s="104"/>
-      <c r="D62" s="115" t="s">
+      <c r="B62" s="90"/>
+      <c r="C62" s="97"/>
+      <c r="D62" s="83" t="s">
         <v>72</v>
       </c>
       <c r="E62" s="31" t="s">
@@ -10718,9 +10718,9 @@
       </c>
     </row>
     <row r="63" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="103"/>
-      <c r="C63" s="104"/>
-      <c r="D63" s="116" t="s">
+      <c r="B63" s="91"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="84" t="s">
         <v>72</v>
       </c>
       <c r="E63" s="31" t="s">
@@ -10864,7 +10864,7 @@
       </c>
     </row>
     <row r="64" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="101" t="s">
+      <c r="B64" s="89" t="s">
         <v>27</v>
       </c>
       <c r="C64" s="92" t="s">
@@ -11008,7 +11008,7 @@
       </c>
     </row>
     <row r="65" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="102"/>
+      <c r="B65" s="90"/>
       <c r="C65" s="92"/>
       <c r="D65" s="44" t="s">
         <v>83</v>
@@ -11148,7 +11148,7 @@
       </c>
     </row>
     <row r="66" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="102"/>
+      <c r="B66" s="90"/>
       <c r="C66" s="92"/>
       <c r="D66" s="44" t="s">
         <v>85</v>
@@ -11288,7 +11288,7 @@
       </c>
     </row>
     <row r="67" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="102"/>
+      <c r="B67" s="90"/>
       <c r="C67" s="92"/>
       <c r="D67" s="44" t="s">
         <v>86</v>
@@ -11428,7 +11428,7 @@
       </c>
     </row>
     <row r="68" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="102"/>
+      <c r="B68" s="90"/>
       <c r="C68" s="92"/>
       <c r="D68" s="44" t="s">
         <v>87</v>
@@ -11568,7 +11568,7 @@
       </c>
     </row>
     <row r="69" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="102"/>
+      <c r="B69" s="90"/>
       <c r="C69" s="92"/>
       <c r="D69" s="44" t="s">
         <v>88</v>
@@ -11706,7 +11706,7 @@
       </c>
     </row>
     <row r="70" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="102"/>
+      <c r="B70" s="90"/>
       <c r="C70" s="92"/>
       <c r="D70" s="44" t="s">
         <v>89</v>
@@ -11779,7 +11779,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="40">
-        <f t="shared" ref="AB70:AQ94" si="11">IF($K70=AB$5,3,IF(OR(AND($H70&lt;=AB$5,AB$5&lt;=$I70),$H70=AB$5),2,IF(AND($F70&lt;=AB$5,AB$5&lt;=$G70),1,0)))</f>
+        <f t="shared" ref="AB70:AQ85" si="11">IF($K70=AB$5,3,IF(OR(AND($H70&lt;=AB$5,AB$5&lt;=$I70),$H70=AB$5),2,IF(AND($F70&lt;=AB$5,AB$5&lt;=$G70),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC70" s="40">
@@ -11844,7 +11844,7 @@
       </c>
     </row>
     <row r="71" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="102"/>
+      <c r="B71" s="90"/>
       <c r="C71" s="92"/>
       <c r="D71" s="44" t="s">
         <v>90</v>
@@ -11857,7 +11857,7 @@
       <c r="J71" s="34"/>
       <c r="K71" s="35"/>
       <c r="M71" s="39">
-        <f t="shared" ref="M71:AB94" si="12">IF($K71=M$5,3,IF(OR(AND($H71&lt;=M$5,M$5&lt;=$I71),$H71=M$5),2,IF(AND($F71&lt;=M$5,M$5&lt;=$G71),1,0)))</f>
+        <f t="shared" ref="M71:AB86" si="12">IF($K71=M$5,3,IF(OR(AND($H71&lt;=M$5,M$5&lt;=$I71),$H71=M$5),2,IF(AND($F71&lt;=M$5,M$5&lt;=$G71),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N71" s="40">
@@ -11982,7 +11982,7 @@
       </c>
     </row>
     <row r="72" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="102"/>
+      <c r="B72" s="90"/>
       <c r="C72" s="92"/>
       <c r="D72" s="44" t="s">
         <v>91</v>
@@ -12120,7 +12120,7 @@
       </c>
     </row>
     <row r="73" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="102"/>
+      <c r="B73" s="90"/>
       <c r="C73" s="92"/>
       <c r="D73" s="44" t="s">
         <v>92</v>
@@ -12258,7 +12258,7 @@
       </c>
     </row>
     <row r="74" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="102"/>
+      <c r="B74" s="90"/>
       <c r="C74" s="92"/>
       <c r="D74" s="44" t="s">
         <v>93</v>
@@ -12396,9 +12396,9 @@
       </c>
     </row>
     <row r="75" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="102"/>
+      <c r="B75" s="90"/>
       <c r="C75" s="92"/>
-      <c r="D75" s="111" t="s">
+      <c r="D75" s="79" t="s">
         <v>94</v>
       </c>
       <c r="E75" s="31"/>
@@ -12534,7 +12534,7 @@
       </c>
     </row>
     <row r="76" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="102"/>
+      <c r="B76" s="90"/>
       <c r="C76" s="92"/>
       <c r="D76" s="50" t="s">
         <v>95</v>
@@ -12672,7 +12672,7 @@
       </c>
     </row>
     <row r="77" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="102"/>
+      <c r="B77" s="90"/>
       <c r="C77" s="92"/>
       <c r="D77" s="45" t="s">
         <v>57</v>
@@ -12816,7 +12816,7 @@
       </c>
     </row>
     <row r="78" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="102"/>
+      <c r="B78" s="90"/>
       <c r="C78" s="92"/>
       <c r="D78" s="60" t="s">
         <v>48</v>
@@ -12958,7 +12958,7 @@
       </c>
     </row>
     <row r="79" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="102"/>
+      <c r="B79" s="90"/>
       <c r="C79" s="92"/>
       <c r="D79" s="46" t="s">
         <v>21</v>
@@ -13098,9 +13098,9 @@
       </c>
     </row>
     <row r="80" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="102"/>
+      <c r="B80" s="90"/>
       <c r="C80" s="92"/>
-      <c r="D80" s="118" t="s">
+      <c r="D80" s="86" t="s">
         <v>96</v>
       </c>
       <c r="E80" s="31" t="s">
@@ -13238,9 +13238,9 @@
       </c>
     </row>
     <row r="81" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="102"/>
+      <c r="B81" s="90"/>
       <c r="C81" s="92"/>
-      <c r="D81" s="118" t="s">
+      <c r="D81" s="86" t="s">
         <v>96</v>
       </c>
       <c r="E81" s="31" t="s">
@@ -13378,9 +13378,9 @@
       </c>
     </row>
     <row r="82" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="102"/>
+      <c r="B82" s="90"/>
       <c r="C82" s="92"/>
-      <c r="D82" s="117" t="s">
+      <c r="D82" s="85" t="s">
         <v>96</v>
       </c>
       <c r="E82" s="31" t="s">
@@ -13522,7 +13522,7 @@
       </c>
     </row>
     <row r="83" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="101" t="s">
+      <c r="B83" s="89" t="s">
         <v>28</v>
       </c>
       <c r="C83" s="92" t="s">
@@ -13666,9 +13666,9 @@
       </c>
     </row>
     <row r="84" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="102"/>
+      <c r="B84" s="90"/>
       <c r="C84" s="92"/>
-      <c r="D84" s="111" t="s">
+      <c r="D84" s="79" t="s">
         <v>97</v>
       </c>
       <c r="E84" s="31" t="s">
@@ -13806,9 +13806,9 @@
       </c>
     </row>
     <row r="85" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="102"/>
+      <c r="B85" s="90"/>
       <c r="C85" s="92"/>
-      <c r="D85" s="111" t="s">
+      <c r="D85" s="79" t="s">
         <v>97</v>
       </c>
       <c r="E85" s="31" t="s">
@@ -13946,9 +13946,9 @@
       </c>
     </row>
     <row r="86" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="102"/>
+      <c r="B86" s="90"/>
       <c r="C86" s="92"/>
-      <c r="D86" s="111" t="s">
+      <c r="D86" s="79" t="s">
         <v>68</v>
       </c>
       <c r="E86" s="31" t="s">
@@ -14086,9 +14086,9 @@
       </c>
     </row>
     <row r="87" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="102"/>
+      <c r="B87" s="90"/>
       <c r="C87" s="92"/>
-      <c r="D87" s="111" t="s">
+      <c r="D87" s="79" t="s">
         <v>68</v>
       </c>
       <c r="E87" s="31" t="s">
@@ -14226,9 +14226,9 @@
       </c>
     </row>
     <row r="88" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="102"/>
+      <c r="B88" s="90"/>
       <c r="C88" s="92"/>
-      <c r="D88" s="111" t="s">
+      <c r="D88" s="79" t="s">
         <v>68</v>
       </c>
       <c r="E88" s="31" t="s">
@@ -14366,7 +14366,7 @@
       </c>
     </row>
     <row r="89" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="102"/>
+      <c r="B89" s="90"/>
       <c r="C89" s="92"/>
       <c r="D89" s="30" t="s">
         <v>34</v>
@@ -14506,7 +14506,7 @@
       </c>
     </row>
     <row r="90" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="102"/>
+      <c r="B90" s="90"/>
       <c r="C90" s="92"/>
       <c r="D90" s="30" t="s">
         <v>34</v>
@@ -14646,7 +14646,7 @@
       </c>
     </row>
     <row r="91" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="102"/>
+      <c r="B91" s="90"/>
       <c r="C91" s="92"/>
       <c r="D91" s="30" t="s">
         <v>34</v>
@@ -14786,7 +14786,7 @@
       </c>
     </row>
     <row r="92" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="102"/>
+      <c r="B92" s="90"/>
       <c r="C92" s="92"/>
       <c r="D92" s="62" t="s">
         <v>58</v>
@@ -14928,16 +14928,16 @@
       </c>
     </row>
     <row r="93" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="102"/>
+      <c r="B93" s="90"/>
       <c r="C93" s="92"/>
       <c r="D93" s="30" t="s">
         <v>48</v>
       </c>
       <c r="E93" s="31"/>
-      <c r="F93" s="119">
+      <c r="F93" s="87">
         <v>44687</v>
       </c>
-      <c r="G93" s="120">
+      <c r="G93" s="88">
         <v>44687</v>
       </c>
       <c r="H93" s="32"/>
@@ -15070,7 +15070,7 @@
       </c>
     </row>
     <row r="94" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="103"/>
+      <c r="B94" s="91"/>
       <c r="C94" s="92"/>
       <c r="D94" s="51" t="s">
         <v>47</v>
@@ -15214,6 +15214,21 @@
   </sheetData>
   <autoFilter ref="D5:E94" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}"/>
   <mergeCells count="22">
+    <mergeCell ref="Y3:AD3"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="C9:C38"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="B17:B27"/>
+    <mergeCell ref="B28:B38"/>
     <mergeCell ref="B83:B94"/>
     <mergeCell ref="C83:C94"/>
     <mergeCell ref="B39:B48"/>
@@ -15221,21 +15236,6 @@
     <mergeCell ref="B49:B63"/>
     <mergeCell ref="B64:B82"/>
     <mergeCell ref="C64:C82"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="C9:C38"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="B17:B27"/>
-    <mergeCell ref="B28:B38"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="S3:X3"/>
-    <mergeCell ref="Y3:AD3"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="M6:AQ94">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Updated week 8 schedule
</commit_message>
<xml_diff>
--- a/CMSC495_ProjectPlan.xlsx
+++ b/CMSC495_ProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Git/cmsc495_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAA1928-BB37-D749-A663-9BD8869F428A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194349A8-4D7D-B941-9F56-25A1631D3693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22280" yWindow="500" windowWidth="28440" windowHeight="24060" xr2:uid="{A3040AE0-0367-2B43-ADDE-84CCD12855DC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="92">
   <si>
     <t>Year</t>
   </si>
@@ -1348,68 +1348,34 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1435,55 +1401,89 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1880,48 +1880,48 @@
       <c r="D3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="90" t="s">
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="91" t="s">
+      <c r="T3" s="103"/>
+      <c r="U3" s="103"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
+      <c r="X3" s="103"/>
+      <c r="Y3" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="91"/>
-      <c r="AA3" s="91"/>
-      <c r="AB3" s="91"/>
-      <c r="AC3" s="91"/>
-      <c r="AD3" s="91"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
+      <c r="AB3" s="87"/>
+      <c r="AC3" s="87"/>
+      <c r="AD3" s="87"/>
     </row>
     <row r="4" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="83"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="93" t="s">
+      <c r="B4" s="95"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95" t="s">
+      <c r="G4" s="90"/>
+      <c r="H4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97" t="s">
+      <c r="I4" s="92"/>
+      <c r="J4" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="98"/>
+      <c r="K4" s="94"/>
       <c r="M4" s="12" t="str">
         <f>TEXT(M5,"aaa")</f>
         <v>Sun</v>
@@ -2216,13 +2216,13 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="88" t="s">
+      <c r="D6" s="100" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -2375,9 +2375,9 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="87"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="89"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="101"/>
       <c r="E7" s="31" t="s">
         <v>13</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>44636</v>
       </c>
       <c r="M7" s="39">
-        <f t="shared" ref="M7:AB38" si="3">IF($K7=M$5,3,IF(OR(AND($H7&lt;=M$5,M$5&lt;=$I7),$H7=M$5),2,IF(AND($F7&lt;=M$5,M$5&lt;=$G7),1,0)))</f>
+        <f t="shared" ref="M7:AB22" si="3">IF($K7=M$5,3,IF(OR(AND($H7&lt;=M$5,M$5&lt;=$I7),$H7=M$5),2,IF(AND($F7&lt;=M$5,M$5&lt;=$G7),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N7" s="40">
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="AC7" s="40">
-        <f t="shared" ref="AC7:AQ70" si="4">IF($K7=AC$5,3,IF(OR(AND($H7&lt;=AC$5,AC$5&lt;=$I7),$H7=AC$5),2,IF(AND($F7&lt;=AC$5,AC$5&lt;=$G7),1,0)))</f>
+        <f t="shared" ref="AC7:AQ21" si="4">IF($K7=AC$5,3,IF(OR(AND($H7&lt;=AC$5,AC$5&lt;=$I7),$H7=AC$5),2,IF(AND($F7&lt;=AC$5,AC$5&lt;=$G7),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AD7" s="40">
@@ -2528,9 +2528,9 @@
       </c>
     </row>
     <row r="8" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="87"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="89"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="101"/>
       <c r="E8" s="31" t="s">
         <v>15</v>
       </c>
@@ -2678,10 +2678,10 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="106" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="54" t="s">
@@ -2834,8 +2834,8 @@
       </c>
     </row>
     <row r="10" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="77"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="55" t="s">
         <v>48</v>
       </c>
@@ -2986,8 +2986,8 @@
       </c>
     </row>
     <row r="11" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="77"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="107"/>
       <c r="D11" s="55" t="s">
         <v>48</v>
       </c>
@@ -3138,8 +3138,8 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="77"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="107"/>
       <c r="D12" s="56" t="s">
         <v>51</v>
       </c>
@@ -3290,8 +3290,8 @@
       </c>
     </row>
     <row r="13" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="77"/>
-      <c r="C13" s="79"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="107"/>
       <c r="D13" s="57" t="s">
         <v>47</v>
       </c>
@@ -3440,9 +3440,9 @@
       </c>
     </row>
     <row r="14" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="77"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="81" t="s">
+      <c r="B14" s="105"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="109" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="31" t="s">
@@ -3588,9 +3588,9 @@
       </c>
     </row>
     <row r="15" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="77"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="82"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="110"/>
       <c r="E15" s="31" t="s">
         <v>13</v>
       </c>
@@ -3738,9 +3738,9 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="77"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="82"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="110"/>
       <c r="E16" s="31" t="s">
         <v>15</v>
       </c>
@@ -3888,10 +3888,10 @@
       </c>
     </row>
     <row r="17" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="107"/>
       <c r="D17" s="58" t="s">
         <v>60</v>
       </c>
@@ -4042,8 +4042,8 @@
       </c>
     </row>
     <row r="18" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="77"/>
-      <c r="C18" s="79"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="107"/>
       <c r="D18" s="59" t="s">
         <v>62</v>
       </c>
@@ -4194,8 +4194,8 @@
       </c>
     </row>
     <row r="19" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="77"/>
-      <c r="C19" s="79"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="107"/>
       <c r="D19" s="60" t="s">
         <v>44</v>
       </c>
@@ -4346,8 +4346,8 @@
       </c>
     </row>
     <row r="20" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="77"/>
-      <c r="C20" s="79"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="60" t="s">
         <v>45</v>
       </c>
@@ -4498,8 +4498,8 @@
       </c>
     </row>
     <row r="21" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="77"/>
-      <c r="C21" s="79"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="107"/>
       <c r="D21" s="60" t="s">
         <v>61</v>
       </c>
@@ -4650,8 +4650,8 @@
       </c>
     </row>
     <row r="22" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="77"/>
-      <c r="C22" s="79"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="107"/>
       <c r="D22" s="61" t="s">
         <v>63</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="40">
-        <f t="shared" ref="AB22:AQ84" si="5">IF($K22=AB$5,3,IF(OR(AND($H22&lt;=AB$5,AB$5&lt;=$I22),$H22=AB$5),2,IF(AND($F22&lt;=AB$5,AB$5&lt;=$G22),1,0)))</f>
+        <f t="shared" ref="AB22:AQ37" si="5">IF($K22=AB$5,3,IF(OR(AND($H22&lt;=AB$5,AB$5&lt;=$I22),$H22=AB$5),2,IF(AND($F22&lt;=AB$5,AB$5&lt;=$G22),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC22" s="40">
@@ -4802,8 +4802,8 @@
       </c>
     </row>
     <row r="23" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="77"/>
-      <c r="C23" s="79"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="107"/>
       <c r="D23" s="61" t="s">
         <v>49</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>44651</v>
       </c>
       <c r="M23" s="39">
-        <f t="shared" ref="M23:AB54" si="6">IF($K23=M$5,3,IF(OR(AND($H23&lt;=M$5,M$5&lt;=$I23),$H23=M$5),2,IF(AND($F23&lt;=M$5,M$5&lt;=$G23),1,0)))</f>
+        <f t="shared" ref="M23:AB38" si="6">IF($K23=M$5,3,IF(OR(AND($H23&lt;=M$5,M$5&lt;=$I23),$H23=M$5),2,IF(AND($F23&lt;=M$5,M$5&lt;=$G23),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N23" s="40">
@@ -4954,8 +4954,8 @@
       </c>
     </row>
     <row r="24" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="77"/>
-      <c r="C24" s="79"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="107"/>
       <c r="D24" s="62" t="s">
         <v>52</v>
       </c>
@@ -5106,8 +5106,8 @@
       </c>
     </row>
     <row r="25" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="77"/>
-      <c r="C25" s="79"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="61" t="s">
         <v>47</v>
       </c>
@@ -5256,8 +5256,8 @@
       </c>
     </row>
     <row r="26" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="77"/>
-      <c r="C26" s="79"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="107"/>
       <c r="D26" s="61" t="s">
         <v>58</v>
       </c>
@@ -5408,8 +5408,8 @@
       </c>
     </row>
     <row r="27" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="77"/>
-      <c r="C27" s="79"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="107"/>
       <c r="D27" s="62" t="s">
         <v>17</v>
       </c>
@@ -5560,10 +5560,10 @@
       </c>
     </row>
     <row r="28" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="79"/>
+      <c r="C28" s="107"/>
       <c r="D28" s="58" t="s">
         <v>50</v>
       </c>
@@ -5714,8 +5714,8 @@
       </c>
     </row>
     <row r="29" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="77"/>
-      <c r="C29" s="79"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="107"/>
       <c r="D29" s="60" t="s">
         <v>38</v>
       </c>
@@ -5866,8 +5866,8 @@
       </c>
     </row>
     <row r="30" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="77"/>
-      <c r="C30" s="79"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="107"/>
       <c r="D30" s="60" t="s">
         <v>64</v>
       </c>
@@ -6018,8 +6018,8 @@
       </c>
     </row>
     <row r="31" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="77"/>
-      <c r="C31" s="79"/>
+      <c r="B31" s="105"/>
+      <c r="C31" s="107"/>
       <c r="D31" s="60" t="s">
         <v>39</v>
       </c>
@@ -6170,8 +6170,8 @@
       </c>
     </row>
     <row r="32" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="77"/>
-      <c r="C32" s="79"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="107"/>
       <c r="D32" s="60" t="s">
         <v>40</v>
       </c>
@@ -6322,8 +6322,8 @@
       </c>
     </row>
     <row r="33" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="77"/>
-      <c r="C33" s="79"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="107"/>
       <c r="D33" s="60" t="s">
         <v>65</v>
       </c>
@@ -6474,8 +6474,8 @@
       </c>
     </row>
     <row r="34" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="77"/>
-      <c r="C34" s="79"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="107"/>
       <c r="D34" s="60" t="s">
         <v>66</v>
       </c>
@@ -6626,8 +6626,8 @@
       </c>
     </row>
     <row r="35" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="77"/>
-      <c r="C35" s="79"/>
+      <c r="B35" s="105"/>
+      <c r="C35" s="107"/>
       <c r="D35" s="62" t="s">
         <v>53</v>
       </c>
@@ -6778,8 +6778,8 @@
       </c>
     </row>
     <row r="36" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="77"/>
-      <c r="C36" s="79"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="107"/>
       <c r="D36" s="61" t="s">
         <v>47</v>
       </c>
@@ -6928,8 +6928,8 @@
       </c>
     </row>
     <row r="37" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="77"/>
-      <c r="C37" s="79"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="107"/>
       <c r="D37" s="60" t="s">
         <v>41</v>
       </c>
@@ -7080,8 +7080,8 @@
       </c>
     </row>
     <row r="38" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="77"/>
-      <c r="C38" s="80"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="108"/>
       <c r="D38" s="62" t="s">
         <v>18</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="40">
-        <f t="shared" ref="AB38:AQ84" si="7">IF($K38=AB$5,3,IF(OR(AND($H38&lt;=AB$5,AB$5&lt;=$I38),$H38=AB$5),2,IF(AND($F38&lt;=AB$5,AB$5&lt;=$G38),1,0)))</f>
+        <f t="shared" ref="AB38:AQ53" si="7">IF($K38=AB$5,3,IF(OR(AND($H38&lt;=AB$5,AB$5&lt;=$I38),$H38=AB$5),2,IF(AND($F38&lt;=AB$5,AB$5&lt;=$G38),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC38" s="40">
@@ -7232,10 +7232,10 @@
       </c>
     </row>
     <row r="39" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="73" t="s">
+      <c r="C39" s="118" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="58" t="s">
@@ -7263,7 +7263,7 @@
         <v>44665</v>
       </c>
       <c r="M39" s="39">
-        <f t="shared" ref="M39:AB84" si="8">IF($K39=M$5,3,IF(OR(AND($H39&lt;=M$5,M$5&lt;=$I39),$H39=M$5),2,IF(AND($F39&lt;=M$5,M$5&lt;=$G39),1,0)))</f>
+        <f t="shared" ref="M39:AB54" si="8">IF($K39=M$5,3,IF(OR(AND($H39&lt;=M$5,M$5&lt;=$I39),$H39=M$5),2,IF(AND($F39&lt;=M$5,M$5&lt;=$G39),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N39" s="40">
@@ -7388,8 +7388,8 @@
       </c>
     </row>
     <row r="40" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="72"/>
-      <c r="C40" s="73"/>
+      <c r="B40" s="117"/>
+      <c r="C40" s="118"/>
       <c r="D40" s="59" t="s">
         <v>68</v>
       </c>
@@ -7540,8 +7540,8 @@
       </c>
     </row>
     <row r="41" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="72"/>
-      <c r="C41" s="73"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
       <c r="D41" s="59" t="s">
         <v>78</v>
       </c>
@@ -7692,8 +7692,8 @@
       </c>
     </row>
     <row r="42" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="72"/>
-      <c r="C42" s="73"/>
+      <c r="B42" s="117"/>
+      <c r="C42" s="118"/>
       <c r="D42" s="59" t="s">
         <v>79</v>
       </c>
@@ -7844,8 +7844,8 @@
       </c>
     </row>
     <row r="43" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="72"/>
-      <c r="C43" s="73"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="118"/>
       <c r="D43" s="60" t="s">
         <v>80</v>
       </c>
@@ -7996,8 +7996,8 @@
       </c>
     </row>
     <row r="44" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="72"/>
-      <c r="C44" s="73"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="118"/>
       <c r="D44" s="62" t="s">
         <v>54</v>
       </c>
@@ -8148,8 +8148,8 @@
       </c>
     </row>
     <row r="45" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="72"/>
-      <c r="C45" s="73"/>
+      <c r="B45" s="117"/>
+      <c r="C45" s="118"/>
       <c r="D45" s="67" t="s">
         <v>47</v>
       </c>
@@ -8298,8 +8298,8 @@
       </c>
     </row>
     <row r="46" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="72"/>
-      <c r="C46" s="73"/>
+      <c r="B46" s="117"/>
+      <c r="C46" s="118"/>
       <c r="D46" s="62" t="s">
         <v>19</v>
       </c>
@@ -8450,10 +8450,10 @@
       </c>
     </row>
     <row r="47" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="71" t="s">
+      <c r="B47" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="73"/>
+      <c r="C47" s="118"/>
       <c r="D47" s="58" t="s">
         <v>77</v>
       </c>
@@ -8604,8 +8604,8 @@
       </c>
     </row>
     <row r="48" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="72"/>
-      <c r="C48" s="73"/>
+      <c r="B48" s="117"/>
+      <c r="C48" s="118"/>
       <c r="D48" s="60" t="s">
         <v>69</v>
       </c>
@@ -8756,8 +8756,8 @@
       </c>
     </row>
     <row r="49" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="72"/>
-      <c r="C49" s="73"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="118"/>
       <c r="D49" s="60" t="s">
         <v>70</v>
       </c>
@@ -8908,8 +8908,8 @@
       </c>
     </row>
     <row r="50" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="72"/>
-      <c r="C50" s="73"/>
+      <c r="B50" s="117"/>
+      <c r="C50" s="118"/>
       <c r="D50" s="60" t="s">
         <v>72</v>
       </c>
@@ -9060,8 +9060,8 @@
       </c>
     </row>
     <row r="51" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="72"/>
-      <c r="C51" s="73"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="118"/>
       <c r="D51" s="60" t="s">
         <v>73</v>
       </c>
@@ -9212,8 +9212,8 @@
       </c>
     </row>
     <row r="52" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="72"/>
-      <c r="C52" s="73"/>
+      <c r="B52" s="117"/>
+      <c r="C52" s="118"/>
       <c r="D52" s="60" t="s">
         <v>74</v>
       </c>
@@ -9364,8 +9364,8 @@
       </c>
     </row>
     <row r="53" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="72"/>
-      <c r="C53" s="73"/>
+      <c r="B53" s="117"/>
+      <c r="C53" s="118"/>
       <c r="D53" s="60" t="s">
         <v>71</v>
       </c>
@@ -9516,8 +9516,8 @@
       </c>
     </row>
     <row r="54" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="72"/>
-      <c r="C54" s="73"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="118"/>
       <c r="D54" s="60" t="s">
         <v>75</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>0</v>
       </c>
       <c r="AB54" s="40">
-        <f t="shared" ref="AB54:AQ84" si="9">IF($K54=AB$5,3,IF(OR(AND($H54&lt;=AB$5,AB$5&lt;=$I54),$H54=AB$5),2,IF(AND($F54&lt;=AB$5,AB$5&lt;=$G54),1,0)))</f>
+        <f t="shared" ref="AB54:AQ69" si="9">IF($K54=AB$5,3,IF(OR(AND($H54&lt;=AB$5,AB$5&lt;=$I54),$H54=AB$5),2,IF(AND($F54&lt;=AB$5,AB$5&lt;=$G54),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC54" s="40">
@@ -9668,8 +9668,8 @@
       </c>
     </row>
     <row r="55" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="72"/>
-      <c r="C55" s="73"/>
+      <c r="B55" s="117"/>
+      <c r="C55" s="118"/>
       <c r="D55" s="61" t="s">
         <v>76</v>
       </c>
@@ -9695,7 +9695,7 @@
         <v>44672</v>
       </c>
       <c r="M55" s="39">
-        <f t="shared" ref="M55:AB84" si="10">IF($K55=M$5,3,IF(OR(AND($H55&lt;=M$5,M$5&lt;=$I55),$H55=M$5),2,IF(AND($F55&lt;=M$5,M$5&lt;=$G55),1,0)))</f>
+        <f t="shared" ref="M55:AB70" si="10">IF($K55=M$5,3,IF(OR(AND($H55&lt;=M$5,M$5&lt;=$I55),$H55=M$5),2,IF(AND($F55&lt;=M$5,M$5&lt;=$G55),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N55" s="40">
@@ -9820,8 +9820,8 @@
       </c>
     </row>
     <row r="56" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="72"/>
-      <c r="C56" s="73"/>
+      <c r="B56" s="117"/>
+      <c r="C56" s="118"/>
       <c r="D56" s="62" t="s">
         <v>55</v>
       </c>
@@ -9972,8 +9972,8 @@
       </c>
     </row>
     <row r="57" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="72"/>
-      <c r="C57" s="73"/>
+      <c r="B57" s="117"/>
+      <c r="C57" s="118"/>
       <c r="D57" s="61" t="s">
         <v>47</v>
       </c>
@@ -10122,8 +10122,8 @@
       </c>
     </row>
     <row r="58" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="72"/>
-      <c r="C58" s="74"/>
+      <c r="B58" s="117"/>
+      <c r="C58" s="119"/>
       <c r="D58" s="62" t="s">
         <v>20</v>
       </c>
@@ -10274,13 +10274,13 @@
       </c>
     </row>
     <row r="59" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="71" t="s">
+      <c r="B59" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="99" t="s">
+      <c r="C59" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="100" t="s">
+      <c r="D59" s="70" t="s">
         <v>84</v>
       </c>
       <c r="E59" s="31" t="s">
@@ -10430,9 +10430,9 @@
       </c>
     </row>
     <row r="60" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="72"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="101" t="s">
+      <c r="B60" s="117"/>
+      <c r="C60" s="121"/>
+      <c r="D60" s="71" t="s">
         <v>84</v>
       </c>
       <c r="E60" s="31" t="s">
@@ -10582,9 +10582,9 @@
       </c>
     </row>
     <row r="61" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="72"/>
-      <c r="C61" s="75"/>
-      <c r="D61" s="101" t="s">
+      <c r="B61" s="117"/>
+      <c r="C61" s="121"/>
+      <c r="D61" s="71" t="s">
         <v>85</v>
       </c>
       <c r="E61" s="31" t="s">
@@ -10734,9 +10734,9 @@
       </c>
     </row>
     <row r="62" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="72"/>
-      <c r="C62" s="75"/>
-      <c r="D62" s="101" t="s">
+      <c r="B62" s="117"/>
+      <c r="C62" s="121"/>
+      <c r="D62" s="71" t="s">
         <v>85</v>
       </c>
       <c r="E62" s="31" t="s">
@@ -10886,9 +10886,9 @@
       </c>
     </row>
     <row r="63" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="72"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="101" t="s">
+      <c r="B63" s="117"/>
+      <c r="C63" s="121"/>
+      <c r="D63" s="71" t="s">
         <v>86</v>
       </c>
       <c r="E63" s="31" t="s">
@@ -11038,9 +11038,9 @@
       </c>
     </row>
     <row r="64" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="72"/>
-      <c r="C64" s="75"/>
-      <c r="D64" s="101" t="s">
+      <c r="B64" s="117"/>
+      <c r="C64" s="121"/>
+      <c r="D64" s="71" t="s">
         <v>86</v>
       </c>
       <c r="E64" s="31" t="s">
@@ -11190,9 +11190,9 @@
       </c>
     </row>
     <row r="65" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="72"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="101" t="s">
+      <c r="B65" s="117"/>
+      <c r="C65" s="121"/>
+      <c r="D65" s="71" t="s">
         <v>86</v>
       </c>
       <c r="E65" s="31" t="s">
@@ -11342,9 +11342,9 @@
       </c>
     </row>
     <row r="66" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="72"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="101" t="s">
+      <c r="B66" s="117"/>
+      <c r="C66" s="121"/>
+      <c r="D66" s="71" t="s">
         <v>83</v>
       </c>
       <c r="E66" s="31" t="s">
@@ -11494,9 +11494,9 @@
       </c>
     </row>
     <row r="67" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="72"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="102" t="s">
+      <c r="B67" s="117"/>
+      <c r="C67" s="121"/>
+      <c r="D67" s="72" t="s">
         <v>81</v>
       </c>
       <c r="E67" s="31" t="s">
@@ -11646,9 +11646,9 @@
       </c>
     </row>
     <row r="68" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="72"/>
-      <c r="C68" s="75"/>
-      <c r="D68" s="103" t="s">
+      <c r="B68" s="117"/>
+      <c r="C68" s="121"/>
+      <c r="D68" s="73" t="s">
         <v>82</v>
       </c>
       <c r="E68" s="31" t="s">
@@ -11798,9 +11798,9 @@
       </c>
     </row>
     <row r="69" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="72"/>
-      <c r="C69" s="75"/>
-      <c r="D69" s="104" t="s">
+      <c r="B69" s="117"/>
+      <c r="C69" s="121"/>
+      <c r="D69" s="74" t="s">
         <v>56</v>
       </c>
       <c r="E69" s="31" t="s">
@@ -11950,9 +11950,9 @@
       </c>
     </row>
     <row r="70" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="72"/>
-      <c r="C70" s="75"/>
-      <c r="D70" s="105" t="s">
+      <c r="B70" s="117"/>
+      <c r="C70" s="121"/>
+      <c r="D70" s="75" t="s">
         <v>47</v>
       </c>
       <c r="E70" s="31"/>
@@ -12100,9 +12100,9 @@
       </c>
     </row>
     <row r="71" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="72"/>
-      <c r="C71" s="112"/>
-      <c r="D71" s="104" t="s">
+      <c r="B71" s="117"/>
+      <c r="C71" s="122"/>
+      <c r="D71" s="74" t="s">
         <v>21</v>
       </c>
       <c r="E71" s="31" t="s">
@@ -12252,13 +12252,13 @@
       </c>
     </row>
     <row r="72" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="113" t="s">
+      <c r="B72" s="111" t="s">
         <v>28</v>
       </c>
       <c r="C72" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="115" t="s">
+      <c r="D72" s="82" t="s">
         <v>91</v>
       </c>
       <c r="E72" s="31" t="s">
@@ -12274,7 +12274,9 @@
         <v>44683</v>
       </c>
       <c r="I72" s="35"/>
-      <c r="J72" s="34"/>
+      <c r="J72" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="K72" s="35"/>
       <c r="M72" s="39">
         <f t="shared" si="12"/>
@@ -12402,8 +12404,8 @@
       </c>
     </row>
     <row r="73" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116"/>
-      <c r="C73" s="70"/>
+      <c r="B73" s="112"/>
+      <c r="C73" s="102"/>
       <c r="D73" s="69" t="s">
         <v>91</v>
       </c>
@@ -12420,7 +12422,9 @@
         <v>44683</v>
       </c>
       <c r="I73" s="35"/>
-      <c r="J73" s="34"/>
+      <c r="J73" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="K73" s="35"/>
       <c r="M73" s="39">
         <f t="shared" si="12"/>
@@ -12548,8 +12552,8 @@
       </c>
     </row>
     <row r="74" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="116"/>
-      <c r="C74" s="70"/>
+      <c r="B74" s="112"/>
+      <c r="C74" s="102"/>
       <c r="D74" s="69" t="s">
         <v>91</v>
       </c>
@@ -12565,8 +12569,12 @@
       <c r="H74" s="32">
         <v>44683</v>
       </c>
-      <c r="I74" s="35"/>
-      <c r="J74" s="34"/>
+      <c r="I74" s="35">
+        <v>44683</v>
+      </c>
+      <c r="J74" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="K74" s="35"/>
       <c r="M74" s="39">
         <f t="shared" si="12"/>
@@ -12694,8 +12702,8 @@
       </c>
     </row>
     <row r="75" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="116"/>
-      <c r="C75" s="70"/>
+      <c r="B75" s="112"/>
+      <c r="C75" s="102"/>
       <c r="D75" s="69" t="s">
         <v>90</v>
       </c>
@@ -12711,8 +12719,12 @@
       <c r="H75" s="32">
         <v>44683</v>
       </c>
-      <c r="I75" s="35"/>
-      <c r="J75" s="34"/>
+      <c r="I75" s="35">
+        <v>44683</v>
+      </c>
+      <c r="J75" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="K75" s="35"/>
       <c r="M75" s="39">
         <f t="shared" si="12"/>
@@ -12840,8 +12852,8 @@
       </c>
     </row>
     <row r="76" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="116"/>
-      <c r="C76" s="70"/>
+      <c r="B76" s="112"/>
+      <c r="C76" s="102"/>
       <c r="D76" s="69" t="s">
         <v>90</v>
       </c>
@@ -12858,7 +12870,9 @@
         <v>44683</v>
       </c>
       <c r="I76" s="35"/>
-      <c r="J76" s="34"/>
+      <c r="J76" s="34" t="s">
+        <v>14</v>
+      </c>
       <c r="K76" s="35"/>
       <c r="M76" s="39">
         <f t="shared" si="12"/>
@@ -12986,8 +13000,8 @@
       </c>
     </row>
     <row r="77" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="116"/>
-      <c r="C77" s="70"/>
+      <c r="B77" s="112"/>
+      <c r="C77" s="102"/>
       <c r="D77" s="69" t="s">
         <v>90</v>
       </c>
@@ -13004,7 +13018,9 @@
         <v>44683</v>
       </c>
       <c r="I77" s="35"/>
-      <c r="J77" s="34"/>
+      <c r="J77" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="K77" s="35"/>
       <c r="M77" s="39">
         <f t="shared" si="12"/>
@@ -13132,8 +13148,8 @@
       </c>
     </row>
     <row r="78" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="116"/>
-      <c r="C78" s="70"/>
+      <c r="B78" s="112"/>
+      <c r="C78" s="102"/>
       <c r="D78" s="69" t="s">
         <v>89</v>
       </c>
@@ -13148,7 +13164,9 @@
       </c>
       <c r="H78" s="32"/>
       <c r="I78" s="35"/>
-      <c r="J78" s="34"/>
+      <c r="J78" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="K78" s="35"/>
       <c r="M78" s="39">
         <f t="shared" si="12"/>
@@ -13276,9 +13294,9 @@
       </c>
     </row>
     <row r="79" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="116"/>
-      <c r="C79" s="70"/>
-      <c r="D79" s="117" t="s">
+      <c r="B79" s="112"/>
+      <c r="C79" s="102"/>
+      <c r="D79" s="83" t="s">
         <v>87</v>
       </c>
       <c r="E79" s="31" t="s">
@@ -13292,7 +13310,9 @@
       </c>
       <c r="H79" s="32"/>
       <c r="I79" s="35"/>
-      <c r="J79" s="34"/>
+      <c r="J79" s="34" t="s">
+        <v>14</v>
+      </c>
       <c r="K79" s="35"/>
       <c r="M79" s="39">
         <f t="shared" si="12"/>
@@ -13420,9 +13440,9 @@
       </c>
     </row>
     <row r="80" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="116"/>
-      <c r="C80" s="70"/>
-      <c r="D80" s="117" t="s">
+      <c r="B80" s="112"/>
+      <c r="C80" s="102"/>
+      <c r="D80" s="83" t="s">
         <v>87</v>
       </c>
       <c r="E80" s="31" t="s">
@@ -13436,7 +13456,9 @@
       </c>
       <c r="H80" s="32"/>
       <c r="I80" s="35"/>
-      <c r="J80" s="34"/>
+      <c r="J80" s="34" t="s">
+        <v>13</v>
+      </c>
       <c r="K80" s="35"/>
       <c r="M80" s="39">
         <f t="shared" si="12"/>
@@ -13564,9 +13586,9 @@
       </c>
     </row>
     <row r="81" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="116"/>
-      <c r="C81" s="70"/>
-      <c r="D81" s="117" t="s">
+      <c r="B81" s="112"/>
+      <c r="C81" s="102"/>
+      <c r="D81" s="83" t="s">
         <v>87</v>
       </c>
       <c r="E81" s="31" t="s">
@@ -13580,7 +13602,9 @@
       </c>
       <c r="H81" s="32"/>
       <c r="I81" s="35"/>
-      <c r="J81" s="34"/>
+      <c r="J81" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="K81" s="35"/>
       <c r="M81" s="39">
         <f t="shared" si="12"/>
@@ -13708,9 +13732,9 @@
       </c>
     </row>
     <row r="82" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="116"/>
-      <c r="C82" s="70"/>
-      <c r="D82" s="118" t="s">
+      <c r="B82" s="112"/>
+      <c r="C82" s="102"/>
+      <c r="D82" s="84" t="s">
         <v>57</v>
       </c>
       <c r="E82" s="31" t="s">
@@ -13724,7 +13748,9 @@
       </c>
       <c r="H82" s="32"/>
       <c r="I82" s="35"/>
-      <c r="J82" s="34"/>
+      <c r="J82" s="34" t="s">
+        <v>14</v>
+      </c>
       <c r="K82" s="35"/>
       <c r="M82" s="39">
         <f t="shared" si="12"/>
@@ -13852,22 +13878,22 @@
       </c>
     </row>
     <row r="83" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="116"/>
-      <c r="C83" s="70"/>
-      <c r="D83" s="119" t="s">
+      <c r="B83" s="112"/>
+      <c r="C83" s="102"/>
+      <c r="D83" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="E83" s="106"/>
-      <c r="F83" s="107">
+      <c r="E83" s="76"/>
+      <c r="F83" s="77">
         <v>44687</v>
       </c>
-      <c r="G83" s="108">
+      <c r="G83" s="78">
         <v>44687</v>
       </c>
-      <c r="H83" s="109"/>
-      <c r="I83" s="110"/>
-      <c r="J83" s="111"/>
-      <c r="K83" s="110"/>
+      <c r="H83" s="79"/>
+      <c r="I83" s="80"/>
+      <c r="J83" s="81"/>
+      <c r="K83" s="80"/>
       <c r="M83" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13994,9 +14020,9 @@
       </c>
     </row>
     <row r="84" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="120"/>
-      <c r="C84" s="121"/>
-      <c r="D84" s="122" t="s">
+      <c r="B84" s="113"/>
+      <c r="C84" s="115"/>
+      <c r="D84" s="86" t="s">
         <v>88</v>
       </c>
       <c r="E84" s="45" t="s">
@@ -14010,7 +14036,9 @@
       </c>
       <c r="H84" s="48"/>
       <c r="I84" s="49"/>
-      <c r="J84" s="50"/>
+      <c r="J84" s="50" t="s">
+        <v>13</v>
+      </c>
       <c r="K84" s="49"/>
       <c r="M84" s="39">
         <f t="shared" si="12"/>
@@ -14140,21 +14168,6 @@
   </sheetData>
   <autoFilter ref="D5:E84" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}"/>
   <mergeCells count="22">
-    <mergeCell ref="Y3:AD3"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="S3:X3"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="C9:C38"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="B17:B27"/>
-    <mergeCell ref="B28:B38"/>
     <mergeCell ref="B72:B84"/>
     <mergeCell ref="C72:C84"/>
     <mergeCell ref="B39:B46"/>
@@ -14162,6 +14175,21 @@
     <mergeCell ref="B47:B58"/>
     <mergeCell ref="B59:B71"/>
     <mergeCell ref="C59:C71"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="C9:C38"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="B17:B27"/>
+    <mergeCell ref="B28:B38"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="Y3:AD3"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="M6:AQ84">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Final Update week8 schedule
</commit_message>
<xml_diff>
--- a/CMSC495_ProjectPlan.xlsx
+++ b/CMSC495_ProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Git/cmsc495_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194349A8-4D7D-B941-9F56-25A1631D3693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF6DE7C-99B8-0A48-871A-142B80A2A9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22280" yWindow="500" windowWidth="28440" windowHeight="24060" xr2:uid="{A3040AE0-0367-2B43-ADDE-84CCD12855DC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Project_Plan" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Project_Plan!$D$5:$E$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Project_Plan!$D$5:$E$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="92">
   <si>
     <t>Year</t>
   </si>
@@ -359,7 +359,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,14 +426,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="61">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -1051,62 +1045,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1188,13 +1126,13 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1207,7 +1145,7 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1216,7 +1154,7 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
@@ -1227,14 +1165,14 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1249,7 +1187,20 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1257,7 +1208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1347,35 +1298,90 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1401,89 +1407,26 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1821,7 +1764,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}">
-  <dimension ref="A1:AV84"/>
+  <dimension ref="A1:AV83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -1880,48 +1823,48 @@
       <c r="D3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="M3" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="88"/>
-      <c r="S3" s="103" t="s">
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="103"/>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="103"/>
-      <c r="X3" s="103"/>
-      <c r="Y3" s="87" t="s">
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="87"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="87"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
     </row>
     <row r="4" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="95"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="89" t="s">
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="101"/>
+      <c r="H4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="93" t="s">
+      <c r="I4" s="103"/>
+      <c r="J4" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="94"/>
+      <c r="K4" s="105"/>
       <c r="M4" s="12" t="str">
         <f>TEXT(M5,"aaa")</f>
         <v>Sun</v>
@@ -2216,13 +2159,13 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="95" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="31" t="s">
@@ -2375,9 +2318,9 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="99"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="101"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="96"/>
       <c r="E7" s="31" t="s">
         <v>13</v>
       </c>
@@ -2528,9 +2471,9 @@
       </c>
     </row>
     <row r="8" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="99"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="101"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="31" t="s">
         <v>15</v>
       </c>
@@ -2678,10 +2621,10 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="106" t="s">
+      <c r="C9" s="85" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="54" t="s">
@@ -2834,8 +2777,8 @@
       </c>
     </row>
     <row r="10" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="105"/>
-      <c r="C10" s="107"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="55" t="s">
         <v>48</v>
       </c>
@@ -2986,8 +2929,8 @@
       </c>
     </row>
     <row r="11" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="105"/>
-      <c r="C11" s="107"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="55" t="s">
         <v>48</v>
       </c>
@@ -3138,8 +3081,8 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="105"/>
-      <c r="C12" s="107"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="56" t="s">
         <v>51</v>
       </c>
@@ -3290,8 +3233,8 @@
       </c>
     </row>
     <row r="13" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="105"/>
-      <c r="C13" s="107"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="57" t="s">
         <v>47</v>
       </c>
@@ -3440,9 +3383,9 @@
       </c>
     </row>
     <row r="14" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="105"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="109" t="s">
+      <c r="B14" s="84"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="88" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="31" t="s">
@@ -3588,9 +3531,9 @@
       </c>
     </row>
     <row r="15" spans="1:48" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="105"/>
-      <c r="C15" s="107"/>
-      <c r="D15" s="110"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="89"/>
       <c r="E15" s="31" t="s">
         <v>13</v>
       </c>
@@ -3738,9 +3681,9 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="105"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="110"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="89"/>
       <c r="E16" s="31" t="s">
         <v>15</v>
       </c>
@@ -3888,10 +3831,10 @@
       </c>
     </row>
     <row r="17" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="107"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="58" t="s">
         <v>60</v>
       </c>
@@ -4042,8 +3985,8 @@
       </c>
     </row>
     <row r="18" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="105"/>
-      <c r="C18" s="107"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="59" t="s">
         <v>62</v>
       </c>
@@ -4194,8 +4137,8 @@
       </c>
     </row>
     <row r="19" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="105"/>
-      <c r="C19" s="107"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="60" t="s">
         <v>44</v>
       </c>
@@ -4346,8 +4289,8 @@
       </c>
     </row>
     <row r="20" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="105"/>
-      <c r="C20" s="107"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="60" t="s">
         <v>45</v>
       </c>
@@ -4498,8 +4441,8 @@
       </c>
     </row>
     <row r="21" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="105"/>
-      <c r="C21" s="107"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="60" t="s">
         <v>61</v>
       </c>
@@ -4650,8 +4593,8 @@
       </c>
     </row>
     <row r="22" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="105"/>
-      <c r="C22" s="107"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="86"/>
       <c r="D22" s="61" t="s">
         <v>63</v>
       </c>
@@ -4802,8 +4745,8 @@
       </c>
     </row>
     <row r="23" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="105"/>
-      <c r="C23" s="107"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="86"/>
       <c r="D23" s="61" t="s">
         <v>49</v>
       </c>
@@ -4954,8 +4897,8 @@
       </c>
     </row>
     <row r="24" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="105"/>
-      <c r="C24" s="107"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="62" t="s">
         <v>52</v>
       </c>
@@ -5106,8 +5049,8 @@
       </c>
     </row>
     <row r="25" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="105"/>
-      <c r="C25" s="107"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="61" t="s">
         <v>47</v>
       </c>
@@ -5256,8 +5199,8 @@
       </c>
     </row>
     <row r="26" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="105"/>
-      <c r="C26" s="107"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="61" t="s">
         <v>58</v>
       </c>
@@ -5408,8 +5351,8 @@
       </c>
     </row>
     <row r="27" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="105"/>
-      <c r="C27" s="107"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="62" t="s">
         <v>17</v>
       </c>
@@ -5560,10 +5503,10 @@
       </c>
     </row>
     <row r="28" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="107"/>
+      <c r="C28" s="86"/>
       <c r="D28" s="58" t="s">
         <v>50</v>
       </c>
@@ -5714,8 +5657,8 @@
       </c>
     </row>
     <row r="29" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="105"/>
-      <c r="C29" s="107"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="60" t="s">
         <v>38</v>
       </c>
@@ -5866,8 +5809,8 @@
       </c>
     </row>
     <row r="30" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="105"/>
-      <c r="C30" s="107"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="60" t="s">
         <v>64</v>
       </c>
@@ -6018,8 +5961,8 @@
       </c>
     </row>
     <row r="31" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="105"/>
-      <c r="C31" s="107"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="60" t="s">
         <v>39</v>
       </c>
@@ -6170,8 +6113,8 @@
       </c>
     </row>
     <row r="32" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="105"/>
-      <c r="C32" s="107"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="60" t="s">
         <v>40</v>
       </c>
@@ -6322,8 +6265,8 @@
       </c>
     </row>
     <row r="33" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="105"/>
-      <c r="C33" s="107"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="60" t="s">
         <v>65</v>
       </c>
@@ -6474,8 +6417,8 @@
       </c>
     </row>
     <row r="34" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="105"/>
-      <c r="C34" s="107"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="86"/>
       <c r="D34" s="60" t="s">
         <v>66</v>
       </c>
@@ -6626,8 +6569,8 @@
       </c>
     </row>
     <row r="35" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="105"/>
-      <c r="C35" s="107"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="86"/>
       <c r="D35" s="62" t="s">
         <v>53</v>
       </c>
@@ -6778,8 +6721,8 @@
       </c>
     </row>
     <row r="36" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="105"/>
-      <c r="C36" s="107"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="86"/>
       <c r="D36" s="61" t="s">
         <v>47</v>
       </c>
@@ -6928,8 +6871,8 @@
       </c>
     </row>
     <row r="37" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="105"/>
-      <c r="C37" s="107"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="86"/>
       <c r="D37" s="60" t="s">
         <v>41</v>
       </c>
@@ -7080,8 +7023,8 @@
       </c>
     </row>
     <row r="38" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="105"/>
-      <c r="C38" s="108"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="87"/>
       <c r="D38" s="62" t="s">
         <v>18</v>
       </c>
@@ -7232,10 +7175,10 @@
       </c>
     </row>
     <row r="39" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="118" t="s">
+      <c r="C39" s="78" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="58" t="s">
@@ -7388,8 +7331,8 @@
       </c>
     </row>
     <row r="40" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="117"/>
-      <c r="C40" s="118"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="59" t="s">
         <v>68</v>
       </c>
@@ -7540,8 +7483,8 @@
       </c>
     </row>
     <row r="41" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="78"/>
       <c r="D41" s="59" t="s">
         <v>78</v>
       </c>
@@ -7692,8 +7635,8 @@
       </c>
     </row>
     <row r="42" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="117"/>
-      <c r="C42" s="118"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="59" t="s">
         <v>79</v>
       </c>
@@ -7844,8 +7787,8 @@
       </c>
     </row>
     <row r="43" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="117"/>
-      <c r="C43" s="118"/>
+      <c r="B43" s="77"/>
+      <c r="C43" s="78"/>
       <c r="D43" s="60" t="s">
         <v>80</v>
       </c>
@@ -7996,8 +7939,8 @@
       </c>
     </row>
     <row r="44" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="117"/>
-      <c r="C44" s="118"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="78"/>
       <c r="D44" s="62" t="s">
         <v>54</v>
       </c>
@@ -8148,8 +8091,8 @@
       </c>
     </row>
     <row r="45" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="117"/>
-      <c r="C45" s="118"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="67" t="s">
         <v>47</v>
       </c>
@@ -8298,8 +8241,8 @@
       </c>
     </row>
     <row r="46" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="117"/>
-      <c r="C46" s="118"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="78"/>
       <c r="D46" s="62" t="s">
         <v>19</v>
       </c>
@@ -8450,10 +8393,10 @@
       </c>
     </row>
     <row r="47" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="116" t="s">
+      <c r="B47" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="118"/>
+      <c r="C47" s="78"/>
       <c r="D47" s="58" t="s">
         <v>77</v>
       </c>
@@ -8604,8 +8547,8 @@
       </c>
     </row>
     <row r="48" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="117"/>
-      <c r="C48" s="118"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="78"/>
       <c r="D48" s="60" t="s">
         <v>69</v>
       </c>
@@ -8756,8 +8699,8 @@
       </c>
     </row>
     <row r="49" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="117"/>
-      <c r="C49" s="118"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="78"/>
       <c r="D49" s="60" t="s">
         <v>70</v>
       </c>
@@ -8908,8 +8851,8 @@
       </c>
     </row>
     <row r="50" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="117"/>
-      <c r="C50" s="118"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="78"/>
       <c r="D50" s="60" t="s">
         <v>72</v>
       </c>
@@ -9060,8 +9003,8 @@
       </c>
     </row>
     <row r="51" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="117"/>
-      <c r="C51" s="118"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="78"/>
       <c r="D51" s="60" t="s">
         <v>73</v>
       </c>
@@ -9212,8 +9155,8 @@
       </c>
     </row>
     <row r="52" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="117"/>
-      <c r="C52" s="118"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="78"/>
       <c r="D52" s="60" t="s">
         <v>74</v>
       </c>
@@ -9364,8 +9307,8 @@
       </c>
     </row>
     <row r="53" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="117"/>
-      <c r="C53" s="118"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="78"/>
       <c r="D53" s="60" t="s">
         <v>71</v>
       </c>
@@ -9516,8 +9459,8 @@
       </c>
     </row>
     <row r="54" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="117"/>
-      <c r="C54" s="118"/>
+      <c r="B54" s="77"/>
+      <c r="C54" s="78"/>
       <c r="D54" s="60" t="s">
         <v>75</v>
       </c>
@@ -9668,8 +9611,8 @@
       </c>
     </row>
     <row r="55" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="117"/>
-      <c r="C55" s="118"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="78"/>
       <c r="D55" s="61" t="s">
         <v>76</v>
       </c>
@@ -9820,8 +9763,8 @@
       </c>
     </row>
     <row r="56" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="117"/>
-      <c r="C56" s="118"/>
+      <c r="B56" s="77"/>
+      <c r="C56" s="78"/>
       <c r="D56" s="62" t="s">
         <v>55</v>
       </c>
@@ -9972,8 +9915,8 @@
       </c>
     </row>
     <row r="57" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="117"/>
-      <c r="C57" s="118"/>
+      <c r="B57" s="77"/>
+      <c r="C57" s="78"/>
       <c r="D57" s="61" t="s">
         <v>47</v>
       </c>
@@ -10122,8 +10065,8 @@
       </c>
     </row>
     <row r="58" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="117"/>
-      <c r="C58" s="119"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="79"/>
       <c r="D58" s="62" t="s">
         <v>20</v>
       </c>
@@ -10274,13 +10217,13 @@
       </c>
     </row>
     <row r="59" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="116" t="s">
+      <c r="B59" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="120" t="s">
+      <c r="C59" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="70" t="s">
+      <c r="D59" s="69" t="s">
         <v>84</v>
       </c>
       <c r="E59" s="31" t="s">
@@ -10430,9 +10373,9 @@
       </c>
     </row>
     <row r="60" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="117"/>
-      <c r="C60" s="121"/>
-      <c r="D60" s="71" t="s">
+      <c r="B60" s="77"/>
+      <c r="C60" s="81"/>
+      <c r="D60" s="70" t="s">
         <v>84</v>
       </c>
       <c r="E60" s="31" t="s">
@@ -10582,9 +10525,9 @@
       </c>
     </row>
     <row r="61" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="117"/>
-      <c r="C61" s="121"/>
-      <c r="D61" s="71" t="s">
+      <c r="B61" s="77"/>
+      <c r="C61" s="81"/>
+      <c r="D61" s="70" t="s">
         <v>85</v>
       </c>
       <c r="E61" s="31" t="s">
@@ -10734,9 +10677,9 @@
       </c>
     </row>
     <row r="62" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="117"/>
-      <c r="C62" s="121"/>
-      <c r="D62" s="71" t="s">
+      <c r="B62" s="77"/>
+      <c r="C62" s="81"/>
+      <c r="D62" s="70" t="s">
         <v>85</v>
       </c>
       <c r="E62" s="31" t="s">
@@ -10886,9 +10829,9 @@
       </c>
     </row>
     <row r="63" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="117"/>
-      <c r="C63" s="121"/>
-      <c r="D63" s="71" t="s">
+      <c r="B63" s="77"/>
+      <c r="C63" s="81"/>
+      <c r="D63" s="70" t="s">
         <v>86</v>
       </c>
       <c r="E63" s="31" t="s">
@@ -11038,9 +10981,9 @@
       </c>
     </row>
     <row r="64" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="117"/>
-      <c r="C64" s="121"/>
-      <c r="D64" s="71" t="s">
+      <c r="B64" s="77"/>
+      <c r="C64" s="81"/>
+      <c r="D64" s="70" t="s">
         <v>86</v>
       </c>
       <c r="E64" s="31" t="s">
@@ -11190,9 +11133,9 @@
       </c>
     </row>
     <row r="65" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="117"/>
-      <c r="C65" s="121"/>
-      <c r="D65" s="71" t="s">
+      <c r="B65" s="77"/>
+      <c r="C65" s="81"/>
+      <c r="D65" s="70" t="s">
         <v>86</v>
       </c>
       <c r="E65" s="31" t="s">
@@ -11342,9 +11285,9 @@
       </c>
     </row>
     <row r="66" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="117"/>
-      <c r="C66" s="121"/>
-      <c r="D66" s="71" t="s">
+      <c r="B66" s="77"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="70" t="s">
         <v>83</v>
       </c>
       <c r="E66" s="31" t="s">
@@ -11494,9 +11437,9 @@
       </c>
     </row>
     <row r="67" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="117"/>
-      <c r="C67" s="121"/>
-      <c r="D67" s="72" t="s">
+      <c r="B67" s="77"/>
+      <c r="C67" s="81"/>
+      <c r="D67" s="71" t="s">
         <v>81</v>
       </c>
       <c r="E67" s="31" t="s">
@@ -11646,9 +11589,9 @@
       </c>
     </row>
     <row r="68" spans="2:43" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="117"/>
-      <c r="C68" s="121"/>
-      <c r="D68" s="73" t="s">
+      <c r="B68" s="77"/>
+      <c r="C68" s="81"/>
+      <c r="D68" s="72" t="s">
         <v>82</v>
       </c>
       <c r="E68" s="31" t="s">
@@ -11798,9 +11741,9 @@
       </c>
     </row>
     <row r="69" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="117"/>
-      <c r="C69" s="121"/>
-      <c r="D69" s="74" t="s">
+      <c r="B69" s="77"/>
+      <c r="C69" s="81"/>
+      <c r="D69" s="73" t="s">
         <v>56</v>
       </c>
       <c r="E69" s="31" t="s">
@@ -11950,9 +11893,9 @@
       </c>
     </row>
     <row r="70" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="117"/>
-      <c r="C70" s="121"/>
-      <c r="D70" s="75" t="s">
+      <c r="B70" s="77"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="74" t="s">
         <v>47</v>
       </c>
       <c r="E70" s="31"/>
@@ -12035,7 +11978,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="40">
-        <f t="shared" ref="AB70:AQ84" si="11">IF($K70=AB$5,3,IF(OR(AND($H70&lt;=AB$5,AB$5&lt;=$I70),$H70=AB$5),2,IF(AND($F70&lt;=AB$5,AB$5&lt;=$G70),1,0)))</f>
+        <f t="shared" ref="AB70:AQ83" si="11">IF($K70=AB$5,3,IF(OR(AND($H70&lt;=AB$5,AB$5&lt;=$I70),$H70=AB$5),2,IF(AND($F70&lt;=AB$5,AB$5&lt;=$G70),1,0)))</f>
         <v>0</v>
       </c>
       <c r="AC70" s="40">
@@ -12100,9 +12043,9 @@
       </c>
     </row>
     <row r="71" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="117"/>
-      <c r="C71" s="122"/>
-      <c r="D71" s="74" t="s">
+      <c r="B71" s="77"/>
+      <c r="C71" s="82"/>
+      <c r="D71" s="73" t="s">
         <v>21</v>
       </c>
       <c r="E71" s="31" t="s">
@@ -12127,7 +12070,7 @@
         <v>44679</v>
       </c>
       <c r="M71" s="39">
-        <f t="shared" ref="M71:AB84" si="12">IF($K71=M$5,3,IF(OR(AND($H71&lt;=M$5,M$5&lt;=$I71),$H71=M$5),2,IF(AND($F71&lt;=M$5,M$5&lt;=$G71),1,0)))</f>
+        <f t="shared" ref="M71:AB83" si="12">IF($K71=M$5,3,IF(OR(AND($H71&lt;=M$5,M$5&lt;=$I71),$H71=M$5),2,IF(AND($F71&lt;=M$5,M$5&lt;=$G71),1,0)))</f>
         <v>0</v>
       </c>
       <c r="N71" s="40">
@@ -12252,13 +12195,13 @@
       </c>
     </row>
     <row r="72" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="111" t="s">
+      <c r="B72" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="C72" s="114" t="s">
+      <c r="C72" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="82" t="s">
+      <c r="D72" s="108" t="s">
         <v>91</v>
       </c>
       <c r="E72" s="31" t="s">
@@ -12273,11 +12216,15 @@
       <c r="H72" s="32">
         <v>44683</v>
       </c>
-      <c r="I72" s="35"/>
+      <c r="I72" s="35">
+        <v>44685</v>
+      </c>
       <c r="J72" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K72" s="35"/>
+      <c r="K72" s="35">
+        <v>44684</v>
+      </c>
       <c r="M72" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12288,11 +12235,11 @@
       </c>
       <c r="O72" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P72" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q72" s="40">
         <f t="shared" si="12"/>
@@ -12404,9 +12351,9 @@
       </c>
     </row>
     <row r="73" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
-      <c r="C73" s="102"/>
-      <c r="D73" s="69" t="s">
+      <c r="B73" s="109"/>
+      <c r="C73" s="75"/>
+      <c r="D73" s="71" t="s">
         <v>91</v>
       </c>
       <c r="E73" s="31" t="s">
@@ -12421,11 +12368,15 @@
       <c r="H73" s="32">
         <v>44683</v>
       </c>
-      <c r="I73" s="35"/>
+      <c r="I73" s="35">
+        <v>44685</v>
+      </c>
       <c r="J73" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K73" s="35"/>
+      <c r="K73" s="35">
+        <v>44684</v>
+      </c>
       <c r="M73" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12436,11 +12387,11 @@
       </c>
       <c r="O73" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P73" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q73" s="40">
         <f t="shared" si="12"/>
@@ -12552,9 +12503,9 @@
       </c>
     </row>
     <row r="74" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
-      <c r="C74" s="102"/>
-      <c r="D74" s="69" t="s">
+      <c r="B74" s="109"/>
+      <c r="C74" s="75"/>
+      <c r="D74" s="71" t="s">
         <v>91</v>
       </c>
       <c r="E74" s="31" t="s">
@@ -12575,7 +12526,9 @@
       <c r="J74" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K74" s="35"/>
+      <c r="K74" s="35">
+        <v>44684</v>
+      </c>
       <c r="M74" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12586,7 +12539,7 @@
       </c>
       <c r="O74" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P74" s="40">
         <f t="shared" si="12"/>
@@ -12702,9 +12655,9 @@
       </c>
     </row>
     <row r="75" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="112"/>
-      <c r="C75" s="102"/>
-      <c r="D75" s="69" t="s">
+      <c r="B75" s="109"/>
+      <c r="C75" s="75"/>
+      <c r="D75" s="71" t="s">
         <v>90</v>
       </c>
       <c r="E75" s="31" t="s">
@@ -12725,7 +12678,9 @@
       <c r="J75" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K75" s="35"/>
+      <c r="K75" s="35">
+        <v>44685</v>
+      </c>
       <c r="M75" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12740,7 +12695,7 @@
       </c>
       <c r="P75" s="40">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q75" s="40">
         <f t="shared" si="12"/>
@@ -12852,9 +12807,9 @@
       </c>
     </row>
     <row r="76" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="112"/>
-      <c r="C76" s="102"/>
-      <c r="D76" s="69" t="s">
+      <c r="B76" s="109"/>
+      <c r="C76" s="75"/>
+      <c r="D76" s="71" t="s">
         <v>90</v>
       </c>
       <c r="E76" s="31" t="s">
@@ -12867,24 +12822,28 @@
         <v>44684</v>
       </c>
       <c r="H76" s="32">
-        <v>44683</v>
-      </c>
-      <c r="I76" s="35"/>
+        <v>44684</v>
+      </c>
+      <c r="I76" s="35">
+        <v>44684</v>
+      </c>
       <c r="J76" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K76" s="35"/>
+      <c r="K76" s="35">
+        <v>44684</v>
+      </c>
       <c r="M76" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N76" s="40">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O76" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P76" s="40">
         <f t="shared" si="12"/>
@@ -13000,9 +12959,9 @@
       </c>
     </row>
     <row r="77" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
-      <c r="C77" s="102"/>
-      <c r="D77" s="69" t="s">
+      <c r="B77" s="109"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="71" t="s">
         <v>90</v>
       </c>
       <c r="E77" s="31" t="s">
@@ -13017,11 +12976,15 @@
       <c r="H77" s="32">
         <v>44683</v>
       </c>
-      <c r="I77" s="35"/>
+      <c r="I77" s="35">
+        <v>44684</v>
+      </c>
       <c r="J77" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K77" s="35"/>
+      <c r="K77" s="35">
+        <v>44684</v>
+      </c>
       <c r="M77" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13032,7 +12995,7 @@
       </c>
       <c r="O77" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P77" s="40">
         <f t="shared" si="12"/>
@@ -13148,9 +13111,9 @@
       </c>
     </row>
     <row r="78" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
-      <c r="C78" s="102"/>
-      <c r="D78" s="69" t="s">
+      <c r="B78" s="109"/>
+      <c r="C78" s="75"/>
+      <c r="D78" s="71" t="s">
         <v>89</v>
       </c>
       <c r="E78" s="31" t="s">
@@ -13162,12 +13125,18 @@
       <c r="G78" s="44">
         <v>44685</v>
       </c>
-      <c r="H78" s="32"/>
-      <c r="I78" s="35"/>
+      <c r="H78" s="32">
+        <v>44684</v>
+      </c>
+      <c r="I78" s="35">
+        <v>44684</v>
+      </c>
       <c r="J78" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K78" s="35"/>
+      <c r="K78" s="35">
+        <v>44684</v>
+      </c>
       <c r="M78" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13178,7 +13147,7 @@
       </c>
       <c r="O78" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P78" s="40">
         <f t="shared" si="12"/>
@@ -13294,9 +13263,9 @@
       </c>
     </row>
     <row r="79" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
-      <c r="C79" s="102"/>
-      <c r="D79" s="83" t="s">
+      <c r="B79" s="109"/>
+      <c r="C79" s="75"/>
+      <c r="D79" s="110" t="s">
         <v>87</v>
       </c>
       <c r="E79" s="31" t="s">
@@ -13308,12 +13277,18 @@
       <c r="G79" s="44">
         <v>44685</v>
       </c>
-      <c r="H79" s="32"/>
-      <c r="I79" s="35"/>
+      <c r="H79" s="32">
+        <v>44685</v>
+      </c>
+      <c r="I79" s="35">
+        <v>44685</v>
+      </c>
       <c r="J79" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K79" s="35"/>
+      <c r="K79" s="35">
+        <v>44685</v>
+      </c>
       <c r="M79" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13328,7 +13303,7 @@
       </c>
       <c r="P79" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q79" s="40">
         <f t="shared" si="12"/>
@@ -13440,9 +13415,9 @@
       </c>
     </row>
     <row r="80" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="112"/>
-      <c r="C80" s="102"/>
-      <c r="D80" s="83" t="s">
+      <c r="B80" s="109"/>
+      <c r="C80" s="75"/>
+      <c r="D80" s="110" t="s">
         <v>87</v>
       </c>
       <c r="E80" s="31" t="s">
@@ -13454,12 +13429,18 @@
       <c r="G80" s="35">
         <v>44685</v>
       </c>
-      <c r="H80" s="32"/>
-      <c r="I80" s="35"/>
+      <c r="H80" s="32">
+        <v>44684</v>
+      </c>
+      <c r="I80" s="35">
+        <v>44684</v>
+      </c>
       <c r="J80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K80" s="35"/>
+      <c r="K80" s="35">
+        <v>44684</v>
+      </c>
       <c r="M80" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13470,7 +13451,7 @@
       </c>
       <c r="O80" s="40">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P80" s="40">
         <f t="shared" si="12"/>
@@ -13586,9 +13567,9 @@
       </c>
     </row>
     <row r="81" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="112"/>
-      <c r="C81" s="102"/>
-      <c r="D81" s="83" t="s">
+      <c r="B81" s="109"/>
+      <c r="C81" s="75"/>
+      <c r="D81" s="110" t="s">
         <v>87</v>
       </c>
       <c r="E81" s="31" t="s">
@@ -13600,12 +13581,18 @@
       <c r="G81" s="35">
         <v>44685</v>
       </c>
-      <c r="H81" s="32"/>
-      <c r="I81" s="35"/>
+      <c r="H81" s="32">
+        <v>44684</v>
+      </c>
+      <c r="I81" s="35">
+        <v>44684</v>
+      </c>
       <c r="J81" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K81" s="35"/>
+      <c r="K81" s="35">
+        <v>44684</v>
+      </c>
       <c r="M81" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13616,7 +13603,7 @@
       </c>
       <c r="O81" s="40">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P81" s="40">
         <f t="shared" si="12"/>
@@ -13732,9 +13719,9 @@
       </c>
     </row>
     <row r="82" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="112"/>
-      <c r="C82" s="102"/>
-      <c r="D82" s="84" t="s">
+      <c r="B82" s="109"/>
+      <c r="C82" s="75"/>
+      <c r="D82" s="111" t="s">
         <v>57</v>
       </c>
       <c r="E82" s="31" t="s">
@@ -13746,12 +13733,18 @@
       <c r="G82" s="35">
         <v>44687</v>
       </c>
-      <c r="H82" s="32"/>
-      <c r="I82" s="35"/>
+      <c r="H82" s="32">
+        <v>44685</v>
+      </c>
+      <c r="I82" s="35">
+        <v>44685</v>
+      </c>
       <c r="J82" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K82" s="35"/>
+      <c r="K82" s="35">
+        <v>44685</v>
+      </c>
       <c r="M82" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13766,7 +13759,7 @@
       </c>
       <c r="P82" s="40">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q82" s="40">
         <f t="shared" si="12"/>
@@ -13879,21 +13872,31 @@
     </row>
     <row r="83" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="112"/>
-      <c r="C83" s="102"/>
-      <c r="D83" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="E83" s="76"/>
-      <c r="F83" s="77">
+      <c r="C83" s="113"/>
+      <c r="D83" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="E83" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F83" s="46">
+        <v>44685</v>
+      </c>
+      <c r="G83" s="47">
         <v>44687</v>
       </c>
-      <c r="G83" s="78">
-        <v>44687</v>
-      </c>
-      <c r="H83" s="79"/>
-      <c r="I83" s="80"/>
-      <c r="J83" s="81"/>
-      <c r="K83" s="80"/>
+      <c r="H83" s="48">
+        <v>44685</v>
+      </c>
+      <c r="I83" s="49">
+        <v>44685</v>
+      </c>
+      <c r="J83" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="K83" s="49">
+        <v>44685</v>
+      </c>
       <c r="M83" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13908,11 +13911,11 @@
       </c>
       <c r="P83" s="40">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q83" s="40">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R83" s="40">
         <f t="shared" si="12"/>
@@ -14015,183 +14018,37 @@
         <v>0</v>
       </c>
       <c r="AQ83" s="41">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="113"/>
-      <c r="C84" s="115"/>
-      <c r="D84" s="86" t="s">
-        <v>88</v>
-      </c>
-      <c r="E84" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F84" s="46">
-        <v>44685</v>
-      </c>
-      <c r="G84" s="47">
-        <v>44687</v>
-      </c>
-      <c r="H84" s="48"/>
-      <c r="I84" s="49"/>
-      <c r="J84" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="K84" s="49"/>
-      <c r="M84" s="39">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="N84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="O84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="P84" s="40">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="Q84" s="40">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="R84" s="40">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="S84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="T84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="U84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="V84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="W84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="X84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Y84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AB84" s="40">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AD84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AG84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AH84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AI84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AJ84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AK84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AM84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AN84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AO84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AP84" s="40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AQ84" s="41">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D5:E84" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}"/>
+  <autoFilter ref="D5:E83" xr:uid="{7FDA5272-6E9B-DE4C-84C9-EA24423944AD}"/>
   <mergeCells count="22">
-    <mergeCell ref="B72:B84"/>
-    <mergeCell ref="C72:C84"/>
+    <mergeCell ref="Y3:AD3"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="S3:X3"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="C9:C38"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="B17:B27"/>
+    <mergeCell ref="B28:B38"/>
+    <mergeCell ref="B72:B83"/>
+    <mergeCell ref="C72:C83"/>
     <mergeCell ref="B39:B46"/>
     <mergeCell ref="C39:C58"/>
     <mergeCell ref="B47:B58"/>
     <mergeCell ref="B59:B71"/>
     <mergeCell ref="C59:C71"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="C9:C38"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="B17:B27"/>
-    <mergeCell ref="B28:B38"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="S3:X3"/>
-    <mergeCell ref="Y3:AD3"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
-  <conditionalFormatting sqref="M6:AQ84">
+  <conditionalFormatting sqref="M6:AQ83">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
@@ -14203,7 +14060,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E84 J6:J84" xr:uid="{7799F778-AC45-524F-B3DE-E4EA92284CF2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J83 E6:E83" xr:uid="{7799F778-AC45-524F-B3DE-E4EA92284CF2}">
       <formula1>$AS$5:$AS$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>